<commit_message>
OO Twenty One - complete game logic
</commit_message>
<xml_diff>
--- a/lesson_5/oo_twenty_one/twenty_one_crc.xlsx
+++ b/lesson_5/oo_twenty_one/twenty_one_crc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswallace/Dropbox/Software-Projects/Launch_School/ls_rb120/lesson_5/oo_twenty_one/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC2E832-ACBE-174C-9A24-31B53721A4F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA19300-9AC0-9D4F-BF22-6859DD38016D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60260" yWindow="-28800" windowWidth="51200" windowHeight="28800" xr2:uid="{49C14D9E-246B-514D-BEB7-B27399C0C8B6}"/>
   </bookViews>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="58">
-  <si>
-    <t>Player</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="72">
   <si>
     <t>display_welcome_message</t>
   </si>
@@ -121,15 +118,6 @@
     <t>Participant</t>
   </si>
   <si>
-    <t>Dealer</t>
-  </si>
-  <si>
-    <t>hit</t>
-  </si>
-  <si>
-    <t>stay</t>
-  </si>
-  <si>
     <t>busted?</t>
   </si>
   <si>
@@ -151,12 +139,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>@name</t>
-  </si>
-  <si>
-    <t>super</t>
-  </si>
-  <si>
     <t>start</t>
   </si>
   <si>
@@ -172,9 +154,6 @@
     <t>dealer_turn</t>
   </si>
   <si>
-    <t>display_initial_cards</t>
-  </si>
-  <si>
     <t>display_participant_cards</t>
   </si>
   <si>
@@ -209,13 +188,76 @@
   </si>
   <si>
     <t>deal_initial_cards</t>
+  </si>
+  <si>
+    <t>display_hand</t>
+  </si>
+  <si>
+    <t>Player &lt; Participant</t>
+  </si>
+  <si>
+    <t>Dealer &lt; Participant</t>
+  </si>
+  <si>
+    <t>display_first_card</t>
+  </si>
+  <si>
+    <t>SUITS</t>
+  </si>
+  <si>
+    <t>FACE_VALUES</t>
+  </si>
+  <si>
+    <t>CARD_VALUES</t>
+  </si>
+  <si>
+    <t>display_hands_for_player</t>
+  </si>
+  <si>
+    <t>display_hand_value</t>
+  </si>
+  <si>
+    <t>Dealer.display_first_card</t>
+  </si>
+  <si>
+    <t>Participant.initialize</t>
+  </si>
+  <si>
+    <t>Player.choose_move</t>
+  </si>
+  <si>
+    <t>Participant.busted?</t>
+  </si>
+  <si>
+    <t>Participant.display_hand</t>
+  </si>
+  <si>
+    <t>Participant.display_hand_value</t>
+  </si>
+  <si>
+    <t>Dealer.choose_move</t>
+  </si>
+  <si>
+    <t>determine_winner</t>
+  </si>
+  <si>
+    <t>max_hand_value</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>Deck.deal_card</t>
+  </si>
+  <si>
+    <t>==</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -255,21 +297,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <strike/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -304,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -328,7 +368,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,15 +393,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
+      <xdr:colOff>716750</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
+      <xdr:rowOff>143264</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>58</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2059748</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>106723</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -374,8 +416,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="6299200" y="3586480"/>
-          <a:ext cx="5466080" cy="7650480"/>
+          <a:off x="6191624" y="3569062"/>
+          <a:ext cx="5462494" cy="7113879"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -404,15 +446,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>802640</xdr:colOff>
+      <xdr:colOff>618992</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1879600</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>128067</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -427,8 +469,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="6289040" y="2885440"/>
-          <a:ext cx="11490960" cy="4094480"/>
+          <a:off x="6093866" y="2852484"/>
+          <a:ext cx="11644726" cy="3913734"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -456,16 +498,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>693697</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>128067</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2113280</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>71120</xdr:rowOff>
+      <xdr:colOff>2062480</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -480,8 +522,114 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="8219440" y="3383280"/>
-          <a:ext cx="3515360" cy="4480560"/>
+          <a:off x="6168571" y="3372437"/>
+          <a:ext cx="5488279" cy="4082869"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1097280</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>111760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1910080</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="37" name="Straight Arrow Connector 36">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C625018C-0425-E741-868A-E629544E07B5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8554720" y="4124960"/>
+          <a:ext cx="9255760" cy="2844800"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1097280</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>111760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2072640</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="43" name="Straight Arrow Connector 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACB3EC71-D451-3840-9274-583FB253CBF0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6583680" y="3942080"/>
+          <a:ext cx="5110480" cy="5527040"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -509,23 +657,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1097280</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1408739</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>111760</xdr:rowOff>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1910080</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2113280</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>96051</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="37" name="Straight Arrow Connector 36">
+        <xdr:cNvPr id="49" name="Straight Arrow Connector 48">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C625018C-0425-E741-868A-E629544E07B5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80207626-4800-214D-A155-B641EC7EA11C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -533,8 +681,644 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="8554720" y="4124960"/>
-          <a:ext cx="9255760" cy="2844800"/>
+          <a:off x="6883613" y="4092004"/>
+          <a:ext cx="4824037" cy="6580265"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1675546</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2113280</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>64034</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="50" name="Straight Arrow Connector 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A32FD69C-A3FA-1940-A352-0956E0288C92}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7150420" y="4303913"/>
+          <a:ext cx="4557230" cy="6517768"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1381760</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>142240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2103120</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>132080</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="53" name="Straight Arrow Connector 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F011DE58-EED2-C84D-B254-8917340A93C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6868160" y="4155440"/>
+          <a:ext cx="4856480" cy="4135120"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1778000</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>172720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2082800</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="54" name="Straight Arrow Connector 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA341127-24E1-C74F-A358-9196C73ABED1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="7264400" y="4368800"/>
+          <a:ext cx="4439920" cy="4074160"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1412240</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2082800</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="67" name="Straight Arrow Connector 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2B9DAE2-0A51-914B-8AAD-A2314FEF5416}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="6898640" y="8280400"/>
+          <a:ext cx="4805680" cy="3566160"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1148080</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2062480</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="77" name="Straight Arrow Connector 76">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B0349588-2ED1-2A48-B5DF-419B4F993079}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6634480" y="3952240"/>
+          <a:ext cx="5049520" cy="6370320"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>528320</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>172720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="86" name="Straight Arrow Connector 85">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBA2A0EF-597E-BA40-9151-7A4B1CA20DFF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="12293600" y="2905760"/>
+          <a:ext cx="1442720" cy="4765040"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>447040</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>40640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="89" name="Straight Arrow Connector 88">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F76EE25-2B87-2E45-A601-E07F4FC03D4D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="12212320" y="2956560"/>
+          <a:ext cx="1574800" cy="7934960"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1219200</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>117395</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2081092</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>132080</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="92" name="Straight Arrow Connector 91">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B88AF133-7C5F-A54E-949B-E04CA6B6BA5C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6694074" y="8932689"/>
+          <a:ext cx="4981388" cy="377542"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1205966</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>117395</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2082800</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>91440</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="95" name="Straight Arrow Connector 94">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAE6E802-9698-9E4D-AB44-EBF01F6B5A3E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="6680840" y="9967899"/>
+          <a:ext cx="4996330" cy="1969759"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>992521</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>90842</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1896932</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>149412</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="109" name="Straight Arrow Connector 108">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07F775B9-44AF-CE46-BF1F-1B5E2B25BD6A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6467395" y="4242355"/>
+          <a:ext cx="11288529" cy="4967813"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1077899</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>85378</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1899663</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>85378</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="111" name="Straight Arrow Connector 110">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47362B10-241C-DD40-8E2A-00821DE08BF8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6552773" y="4236891"/>
+          <a:ext cx="11205882" cy="5880420"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>960504</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>96050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1888991</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>128067</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="114" name="Straight Arrow Connector 113">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8BAF8EF-1C41-924D-82C4-2C925DA67861}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6435378" y="4247563"/>
+          <a:ext cx="11312605" cy="3788655"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -861,10 +1645,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E787865A-2D53-2E40-B8D7-C6AC60E2FBBF}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:O95"/>
+  <dimension ref="A1:O100"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="119" workbookViewId="0">
+      <selection activeCell="L35" sqref="L35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -885,13 +1669,13 @@
     <row r="1" spans="2:15" x14ac:dyDescent="0.2"/>
     <row r="2" spans="2:15" ht="26" x14ac:dyDescent="0.3">
       <c r="B2" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:15" ht="22" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
@@ -899,13 +1683,13 @@
       <c r="F4" s="11"/>
       <c r="G4" s="3"/>
       <c r="H4" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I4" s="11"/>
       <c r="J4" s="11"/>
       <c r="K4" s="3"/>
       <c r="L4" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
@@ -925,160 +1709,173 @@
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="10" t="s">
         <v>12</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>13</v>
       </c>
       <c r="F6" s="10"/>
       <c r="G6" s="3"/>
       <c r="H6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="J6" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>13</v>
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="N6" s="9" t="s">
         <v>12</v>
-      </c>
-      <c r="N6" s="9" t="s">
-        <v>13</v>
       </c>
       <c r="O6" s="3"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M7" s="2"/>
+        <v>5</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>55</v>
+      </c>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="M9" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D11" s="1"/>
       <c r="H11" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="L11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12" s="1"/>
       <c r="H12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="L12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="N12" s="1"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.2"/>
     <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" t="s">
         <v>17</v>
       </c>
-      <c r="D14" t="s">
-        <v>18</v>
-      </c>
       <c r="H14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" t="s">
         <v>17</v>
       </c>
-      <c r="I14" t="s">
-        <v>18</v>
-      </c>
       <c r="L14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M14" t="s">
         <v>17</v>
-      </c>
-      <c r="M14" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.2"/>
     <row r="16" spans="2:15" x14ac:dyDescent="0.2">
       <c r="C16" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D17" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" t="s">
-        <v>8</v>
+        <v>30</v>
+      </c>
+      <c r="E17" t="s">
+        <v>7</v>
       </c>
       <c r="I17" s="1"/>
       <c r="M17" s="1" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D18" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E18" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.2">
       <c r="H19" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M19" s="2"/>
       <c r="N19" s="2"/>
@@ -1086,443 +1883,566 @@
     <row r="20" spans="3:14" x14ac:dyDescent="0.2">
       <c r="H20" s="4"/>
       <c r="I20" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="I21" s="15" t="s">
-        <v>30</v>
+      <c r="I21" t="s">
+        <v>51</v>
       </c>
       <c r="M21" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.2">
       <c r="I22" t="s">
-        <v>31</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M22" s="4"/>
+        <v>59</v>
+      </c>
+      <c r="M22" s="17" t="s">
+        <v>29</v>
+      </c>
       <c r="N22" s="4"/>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D23" s="1"/>
-      <c r="M23" t="s">
-        <v>52</v>
+      <c r="I23" s="15" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C24" s="2" t="s">
-        <v>4</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="I24" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="M24" s="4"/>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D25" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.2"/>
+        <v>2</v>
+      </c>
+      <c r="M25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="I26" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C27" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D28" t="s">
-        <v>41</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="3:14" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="3:14" ht="19" x14ac:dyDescent="0.25">
       <c r="D30" t="s">
-        <v>1</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I30" s="12"/>
+      <c r="J30" s="13"/>
+      <c r="L30" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="M30" s="12"/>
+      <c r="N30" s="12"/>
     </row>
     <row r="31" spans="3:14" ht="19" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>42</v>
-      </c>
-      <c r="H31" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="I31" s="12"/>
-      <c r="J31" s="13"/>
-      <c r="L31" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
-    </row>
-    <row r="32" spans="3:14" ht="19" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+      <c r="H31" s="6"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="3"/>
+      <c r="N31" s="3"/>
+    </row>
+    <row r="32" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D32" t="s">
-        <v>19</v>
-      </c>
-      <c r="H32" s="6"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
+        <v>9</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J32" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L32" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M32" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N32" s="9" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.2">
       <c r="D33" t="s">
-        <v>10</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="J33" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L33" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M33" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="N33" s="9" t="s">
-        <v>13</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I33" s="2"/>
+      <c r="L33" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M33" s="2"/>
+      <c r="N33" s="2"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D34" t="s">
-        <v>2</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="H34" s="2"/>
       <c r="I34" s="2"/>
-      <c r="L34" s="2" t="s">
-        <v>6</v>
-      </c>
+      <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" t="s">
+        <v>49</v>
+      </c>
+      <c r="E35" t="s">
+        <v>48</v>
+      </c>
+      <c r="F35" t="s">
+        <v>47</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D36" t="s">
-        <v>56</v>
-      </c>
-      <c r="E36" t="s">
-        <v>55</v>
-      </c>
-      <c r="F36" t="s">
-        <v>54</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L36" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="H36" t="s">
+        <v>13</v>
+      </c>
+      <c r="I36" s="1"/>
+      <c r="L36" t="s">
+        <v>13</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N36" s="1"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>36</v>
+      </c>
       <c r="D37" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H37" t="s">
         <v>14</v>
       </c>
-      <c r="I37" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="I37" s="1"/>
       <c r="L37" t="s">
         <v>14</v>
       </c>
-      <c r="M37" s="1" t="s">
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>36</v>
+      </c>
+      <c r="D39" t="s">
+        <v>38</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" t="s">
+        <v>17</v>
+      </c>
+      <c r="J39" t="s">
+        <v>61</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M39" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>36</v>
+      </c>
+      <c r="D40" t="s">
+        <v>19</v>
+      </c>
+      <c r="H40" s="2"/>
+      <c r="L40" s="2"/>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="H41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I41" s="2"/>
+      <c r="L41" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M41" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="N41" s="2"/>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
         <v>50</v>
       </c>
-      <c r="N37" s="1"/>
-    </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D38" t="s">
-        <v>45</v>
-      </c>
-      <c r="H38" t="s">
-        <v>15</v>
-      </c>
-      <c r="I38" s="1"/>
-      <c r="L38" t="s">
-        <v>15</v>
-      </c>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
-    </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D39" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D40" t="s">
-        <v>44</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I40" t="s">
-        <v>18</v>
-      </c>
-      <c r="L40" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="M40" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D41" t="s">
-        <v>20</v>
-      </c>
-      <c r="H41" s="2"/>
-      <c r="L41" s="2"/>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H42" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="E42" t="s">
+        <v>70</v>
+      </c>
+      <c r="H42" s="2"/>
       <c r="I42" s="2"/>
-      <c r="L42" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="M42" s="14" t="s">
-        <v>51</v>
-      </c>
+      <c r="L42" s="2"/>
+      <c r="M42" s="14"/>
       <c r="N42" s="2"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="I43" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="M43" s="1"/>
-      <c r="N43" s="1"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="14"/>
+      <c r="N43" s="2"/>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>43</v>
-      </c>
-      <c r="D44" t="s">
-        <v>46</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="E44" t="s">
+        <v>60</v>
+      </c>
+      <c r="I44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>43</v>
-      </c>
-      <c r="D45" t="s">
-        <v>47</v>
+        <v>58</v>
+      </c>
+      <c r="E45" t="s">
+        <v>64</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I45" s="2"/>
       <c r="L45" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>43</v>
-      </c>
-      <c r="D46" t="s">
-        <v>33</v>
+        <v>58</v>
+      </c>
+      <c r="E46" t="s">
+        <v>65</v>
+      </c>
+      <c r="I46" t="s">
+        <v>35</v>
       </c>
       <c r="M46" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="H48" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I48" s="12"/>
-      <c r="J48" s="13"/>
-      <c r="L48" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="M48" s="12"/>
-      <c r="N48" s="12"/>
-    </row>
-    <row r="49" spans="8:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="H49" s="6"/>
-      <c r="I49" s="3"/>
-      <c r="L49" s="6"/>
-      <c r="M49" s="3"/>
-      <c r="N49" s="3"/>
-    </row>
-    <row r="50" spans="8:14" x14ac:dyDescent="0.2">
-      <c r="H50" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="I47" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.2"/>
+    <row r="49" spans="2:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>37</v>
+      </c>
+      <c r="E49" t="s">
+        <v>62</v>
+      </c>
+      <c r="H49" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="I49" s="12"/>
+      <c r="J49" s="13"/>
+      <c r="L49" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="M49" s="12"/>
+      <c r="N49" s="12"/>
+    </row>
+    <row r="50" spans="2:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>37</v>
+      </c>
+      <c r="E50" t="s">
+        <v>70</v>
+      </c>
+      <c r="H50" s="6"/>
+      <c r="I50" s="3"/>
+      <c r="L50" s="6"/>
+      <c r="M50" s="3"/>
+      <c r="N50" s="3"/>
+    </row>
+    <row r="51" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>37</v>
+      </c>
+      <c r="E51" t="s">
+        <v>63</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I51" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I50" s="5" t="s">
+      <c r="J51" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="J50" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L50" s="5" t="s">
+      <c r="L51" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M51" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M50" s="5" t="s">
+      <c r="N51" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="N50" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="51" spans="8:14" x14ac:dyDescent="0.2">
-      <c r="H51" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I51" s="2"/>
-      <c r="L51" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M51" s="2"/>
-      <c r="N51" s="2"/>
-    </row>
-    <row r="52" spans="8:14" x14ac:dyDescent="0.2">
-      <c r="H52" s="2"/>
+    </row>
+    <row r="52" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="H52" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="I52" s="2"/>
-      <c r="L52" s="2"/>
+      <c r="L52" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
     </row>
-    <row r="53" spans="8:14" x14ac:dyDescent="0.2">
-      <c r="H53" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L53" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="54" spans="8:14" x14ac:dyDescent="0.2">
-      <c r="H54" t="s">
-        <v>14</v>
-      </c>
-      <c r="I54" s="1"/>
-      <c r="L54" t="s">
-        <v>14</v>
-      </c>
-      <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
-    </row>
-    <row r="55" spans="8:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>38</v>
+      </c>
+      <c r="D53" t="s">
+        <v>39</v>
+      </c>
+      <c r="H53" s="2"/>
+      <c r="I53" s="2"/>
+      <c r="L53" s="2"/>
+      <c r="M53" s="2"/>
+      <c r="N53" s="2"/>
+    </row>
+    <row r="54" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>38</v>
+      </c>
+      <c r="E54" t="s">
+        <v>66</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L54" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B55" t="s">
+        <v>38</v>
+      </c>
+      <c r="E55" t="s">
+        <v>70</v>
+      </c>
       <c r="H55" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="I55" s="1"/>
       <c r="L55" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="M55" s="1"/>
       <c r="N55" s="1"/>
     </row>
-    <row r="56" spans="8:14" x14ac:dyDescent="0.2"/>
-    <row r="57" spans="8:14" x14ac:dyDescent="0.2">
-      <c r="H57" s="2" t="s">
+    <row r="56" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>38</v>
+      </c>
+      <c r="E56" t="s">
+        <v>63</v>
+      </c>
+      <c r="H56" t="s">
+        <v>14</v>
+      </c>
+      <c r="I56" s="1"/>
+      <c r="L56" t="s">
+        <v>14</v>
+      </c>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+    </row>
+    <row r="57" spans="2:14" x14ac:dyDescent="0.2"/>
+    <row r="58" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
+        <v>39</v>
+      </c>
+      <c r="E58" t="s">
+        <v>64</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I58" t="s">
         <v>17</v>
       </c>
-      <c r="I57" t="s">
+      <c r="J58" t="s">
+        <v>61</v>
+      </c>
+      <c r="L58" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
         <v>39</v>
       </c>
-      <c r="L57" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="58" spans="8:14" x14ac:dyDescent="0.2">
-      <c r="H58" s="2"/>
-      <c r="L58" s="2"/>
-    </row>
-    <row r="59" spans="8:14" x14ac:dyDescent="0.2">
-      <c r="H59" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I59" s="2"/>
-      <c r="L59" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="M59" s="2"/>
-      <c r="N59" s="2"/>
-    </row>
-    <row r="60" spans="8:14" x14ac:dyDescent="0.2">
-      <c r="M60" s="1"/>
-      <c r="N60" s="1"/>
-    </row>
-    <row r="61" spans="8:14" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="8:14" x14ac:dyDescent="0.2">
+      <c r="E59" t="s">
+        <v>65</v>
+      </c>
+      <c r="H59" s="2"/>
+      <c r="L59" s="2"/>
+    </row>
+    <row r="60" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="H60" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I60" s="2"/>
+      <c r="L60" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
+    </row>
+    <row r="61" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>19</v>
+      </c>
+      <c r="D61" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+    </row>
+    <row r="62" spans="2:14" x14ac:dyDescent="0.2">
       <c r="H62" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I62" s="2"/>
       <c r="L62" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M62" s="2"/>
       <c r="N62" s="2"/>
     </row>
-    <row r="63" spans="8:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:14" x14ac:dyDescent="0.2">
       <c r="I63" t="s">
-        <v>33</v>
-      </c>
-      <c r="M63" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="64" spans="8:14" x14ac:dyDescent="0.2"/>
-    <row r="65" x14ac:dyDescent="0.2"/>
-    <row r="66" x14ac:dyDescent="0.2"/>
-    <row r="67" x14ac:dyDescent="0.2"/>
-    <row r="68" x14ac:dyDescent="0.2"/>
-    <row r="69" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+        <v>29</v>
+      </c>
+      <c r="M63" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="64" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="I64" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="65" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I65" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="66" spans="9:9" x14ac:dyDescent="0.2"/>
+    <row r="67" spans="9:9" x14ac:dyDescent="0.2"/>
+    <row r="68" spans="9:9" x14ac:dyDescent="0.2"/>
+    <row r="69" spans="9:9" x14ac:dyDescent="0.2"/>
+    <row r="70" spans="9:9" x14ac:dyDescent="0.2"/>
+    <row r="71" spans="9:9" x14ac:dyDescent="0.2"/>
+    <row r="72" spans="9:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="9:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" spans="9:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="9:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" spans="9:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="9:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="9:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="9:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="9:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="81" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="82" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="83" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="84" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="92" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="93" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="94" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="95" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B4:F4"/>

</xml_diff>

<commit_message>
OO Twenty One - display_hand values, determine_hand_values, busted?, >, ==
</commit_message>
<xml_diff>
--- a/lesson_5/oo_twenty_one/twenty_one_crc.xlsx
+++ b/lesson_5/oo_twenty_one/twenty_one_crc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswallace/Dropbox/Software-Projects/Launch_School/ls_rb120/lesson_5/oo_twenty_one/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA19300-9AC0-9D4F-BF22-6859DD38016D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E90949-677A-D448-ABAE-A2846E7177AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60260" yWindow="-28800" windowWidth="51200" windowHeight="28800" xr2:uid="{49C14D9E-246B-514D-BEB7-B27399C0C8B6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="79">
   <si>
     <t>display_welcome_message</t>
   </si>
@@ -121,9 +121,6 @@
     <t>busted?</t>
   </si>
   <si>
-    <t>total_hand_value</t>
-  </si>
-  <si>
     <t>deal_card</t>
   </si>
   <si>
@@ -136,7 +133,7 @@
     <t>Dealer.new</t>
   </si>
   <si>
-    <t>name</t>
+    <t>@name</t>
   </si>
   <si>
     <t>start</t>
@@ -251,6 +248,30 @@
   </si>
   <si>
     <t>==</t>
+  </si>
+  <si>
+    <t>min_hand_value</t>
+  </si>
+  <si>
+    <t>@hand</t>
+  </si>
+  <si>
+    <t>hand_values</t>
+  </si>
+  <si>
+    <t>name, hand, hand_values</t>
+  </si>
+  <si>
+    <t>@hand_values</t>
+  </si>
+  <si>
+    <t>determine_hand_values</t>
+  </si>
+  <si>
+    <t>TWENTY_ONE_THRESHOLD</t>
+  </si>
+  <si>
+    <t>Game::TWENTY_ONE_THRESHOLD</t>
   </si>
 </sst>
 </file>
@@ -369,8 +390,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,7 +421,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2059748</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>106723</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -453,7 +474,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1879600</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>128067</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -506,7 +527,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2062480</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -559,7 +580,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1910080</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -612,7 +633,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2072640</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -665,7 +686,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2113280</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>96051</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -718,7 +739,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2113280</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>64034</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -771,7 +792,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2103120</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>132080</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -824,7 +845,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2082800</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>46</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -871,13 +892,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1412240</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2082800</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>64</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -930,7 +951,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2062480</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -983,7 +1004,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1036,7 +1057,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>57</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1083,13 +1104,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1219200</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>117395</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2081092</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>132080</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1136,13 +1157,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1205966</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>117395</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2082800</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1195,7 +1216,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1896932</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>149412</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1248,7 +1269,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1899663</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>85378</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1301,7 +1322,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1888991</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>128067</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1336,6 +1357,62 @@
         </a:fillRef>
         <a:effectRef idx="0">
           <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1579496</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>117395</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1921008</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>53362</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="119" name="Straight Arrow Connector 118">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD9236B0-93DA-4145-AB0F-CB7CAF6B49EA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5090672" y="1728908"/>
+          <a:ext cx="8569832" cy="2113109"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="7030A0"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -1645,10 +1722,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E787865A-2D53-2E40-B8D7-C6AC60E2FBBF}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:O100"/>
+  <dimension ref="A1:O101"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="119" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -1754,18 +1831,21 @@
         <v>5</v>
       </c>
       <c r="M7" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>77</v>
+      </c>
+      <c r="M8" t="s">
         <v>55</v>
-      </c>
-      <c r="N7" s="2"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="M8" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">
       <c r="M9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.2">
@@ -1788,13 +1868,13 @@
         <v>13</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="L11" t="s">
         <v>13</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N11" s="1"/>
     </row>
@@ -1806,11 +1886,14 @@
       <c r="H12" t="s">
         <v>14</v>
       </c>
+      <c r="I12" t="s">
+        <v>73</v>
+      </c>
       <c r="L12" t="s">
         <v>14</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N12" s="1"/>
     </row>
@@ -1843,6 +1926,9 @@
       <c r="H16" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="I16" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="L16" s="2" t="s">
         <v>4</v>
       </c>
@@ -1851,23 +1937,28 @@
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>
       </c>
-      <c r="I17" s="1"/>
+      <c r="I17" s="1" t="s">
+        <v>72</v>
+      </c>
       <c r="M17" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" t="s">
         <v>31</v>
       </c>
-      <c r="E18" t="s">
-        <v>32</v>
+      <c r="I18" s="1" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.2">
@@ -1882,8 +1973,11 @@
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.2">
       <c r="H20" s="4"/>
-      <c r="I20" s="15" t="s">
+      <c r="I20" s="16" t="s">
         <v>27</v>
+      </c>
+      <c r="J20" t="s">
+        <v>78</v>
       </c>
       <c r="M20" t="s">
         <v>6</v>
@@ -1891,33 +1985,33 @@
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.2">
       <c r="I21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.2">
       <c r="I22" t="s">
-        <v>59</v>
-      </c>
-      <c r="M22" s="17" t="s">
-        <v>29</v>
+        <v>58</v>
+      </c>
+      <c r="M22" s="16" t="s">
+        <v>28</v>
       </c>
       <c r="N22" s="4"/>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D23" s="1"/>
-      <c r="I23" s="15" t="s">
-        <v>69</v>
+      <c r="I23" s="16" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C24" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I24" s="16" t="s">
-        <v>71</v>
+      <c r="I24" s="17" t="s">
+        <v>70</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>2</v>
@@ -1926,229 +2020,230 @@
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>2</v>
       </c>
       <c r="M25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.2">
       <c r="I26" s="15" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C27" s="2" t="s">
+      <c r="I27" s="16" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C28" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D28" t="s">
-        <v>8</v>
+      <c r="I28" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D30" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="3:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="D30" t="s">
-        <v>36</v>
-      </c>
-      <c r="H30" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="I30" s="12"/>
-      <c r="J30" s="13"/>
-      <c r="L30" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="M30" s="12"/>
-      <c r="N30" s="12"/>
     </row>
     <row r="31" spans="3:14" ht="19" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
+        <v>35</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="I31" s="12"/>
+      <c r="J31" s="13"/>
+      <c r="L31" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="M31" s="12"/>
+      <c r="N31" s="12"/>
+    </row>
+    <row r="32" spans="3:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
         <v>18</v>
       </c>
-      <c r="H31" s="6"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-    </row>
-    <row r="32" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D32" t="s">
-        <v>9</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J32" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="L32" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M32" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N32" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="H32" s="6"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.2">
       <c r="D33" t="s">
+        <v>9</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J33" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L33" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M33" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N33" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D34" t="s">
         <v>1</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="H34" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I33" s="2"/>
-      <c r="L33" s="2" t="s">
+      <c r="I34" s="2"/>
+      <c r="L34" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="L34" s="2"/>
       <c r="M34" s="2"/>
       <c r="N34" s="2"/>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>36</v>
-      </c>
-      <c r="D35" t="s">
-        <v>49</v>
-      </c>
-      <c r="E35" t="s">
-        <v>48</v>
-      </c>
-      <c r="F35" t="s">
-        <v>47</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L35" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="M35" s="2"/>
+      <c r="N35" s="2"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D36" t="s">
-        <v>50</v>
-      </c>
-      <c r="H36" t="s">
-        <v>13</v>
-      </c>
-      <c r="I36" s="1"/>
-      <c r="L36" t="s">
-        <v>13</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N36" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="E36" t="s">
+        <v>47</v>
+      </c>
+      <c r="F36" t="s">
+        <v>46</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D37" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="H37" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I37" s="1"/>
       <c r="L37" t="s">
-        <v>14</v>
-      </c>
-      <c r="M37" s="1"/>
+        <v>13</v>
+      </c>
+      <c r="M37" s="1" t="s">
+        <v>42</v>
+      </c>
       <c r="N37" s="1"/>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D38" t="s">
-        <v>37</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="H38" t="s">
+        <v>14</v>
+      </c>
+      <c r="I38" s="1"/>
+      <c r="L38" t="s">
+        <v>14</v>
+      </c>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
+        <v>35</v>
+      </c>
+      <c r="D39" t="s">
         <v>36</v>
-      </c>
-      <c r="D39" t="s">
-        <v>38</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I39" t="s">
-        <v>17</v>
-      </c>
-      <c r="J39" t="s">
-        <v>61</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M39" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D40" t="s">
+        <v>37</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I40" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" t="s">
+        <v>60</v>
+      </c>
+      <c r="L40" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M40" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>35</v>
+      </c>
+      <c r="D41" t="s">
         <v>19</v>
       </c>
-      <c r="H40" s="2"/>
-      <c r="L40" s="2"/>
-    </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H41" s="2" t="s">
+      <c r="H41" s="2"/>
+      <c r="L41" s="2"/>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="H42" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I41" s="2"/>
-      <c r="L41" s="2" t="s">
+      <c r="I42" s="2"/>
+      <c r="L42" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M41" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="N41" s="2"/>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
-        <v>50</v>
-      </c>
-      <c r="E42" t="s">
-        <v>70</v>
-      </c>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="14"/>
+      <c r="M42" s="14" t="s">
+        <v>43</v>
+      </c>
       <c r="N42" s="2"/>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>49</v>
+      </c>
+      <c r="E43" t="s">
+        <v>69</v>
+      </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
       <c r="L43" s="2"/>
@@ -2156,270 +2251,273 @@
       <c r="N43" s="2"/>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
-        <v>58</v>
-      </c>
-      <c r="E44" t="s">
-        <v>60</v>
-      </c>
-      <c r="I44" s="1"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
+      <c r="H44" s="2"/>
+      <c r="I44" s="2"/>
+      <c r="L44" s="2"/>
+      <c r="M44" s="14"/>
+      <c r="N44" s="2"/>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E45" t="s">
-        <v>64</v>
-      </c>
-      <c r="H45" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I45" s="2"/>
-      <c r="L45" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
+        <v>59</v>
+      </c>
+      <c r="I45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E46" t="s">
-        <v>65</v>
-      </c>
-      <c r="I46" t="s">
-        <v>35</v>
-      </c>
-      <c r="M46" t="s">
+        <v>63</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I46" s="2"/>
+      <c r="L46" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>57</v>
+      </c>
+      <c r="E47" t="s">
+        <v>64</v>
+      </c>
+      <c r="I47" t="s">
+        <v>34</v>
+      </c>
+      <c r="M47" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="I47" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.2"/>
-    <row r="49" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>37</v>
-      </c>
-      <c r="E49" t="s">
-        <v>62</v>
-      </c>
-      <c r="H49" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="I49" s="12"/>
-      <c r="J49" s="13"/>
-      <c r="L49" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="M49" s="12"/>
-      <c r="N49" s="12"/>
-    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="I48" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="49" spans="2:14" x14ac:dyDescent="0.2"/>
     <row r="50" spans="2:14" ht="19" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E50" t="s">
-        <v>70</v>
-      </c>
-      <c r="H50" s="6"/>
-      <c r="I50" s="3"/>
-      <c r="L50" s="6"/>
-      <c r="M50" s="3"/>
-      <c r="N50" s="3"/>
-    </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+      <c r="H50" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="I50" s="12"/>
+      <c r="J50" s="13"/>
+      <c r="L50" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="M50" s="12"/>
+      <c r="N50" s="12"/>
+    </row>
+    <row r="51" spans="2:14" ht="19" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E51" t="s">
-        <v>63</v>
-      </c>
-      <c r="H51" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H51" s="6"/>
+      <c r="I51" s="3"/>
+      <c r="L51" s="6"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+    </row>
+    <row r="52" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>36</v>
+      </c>
+      <c r="E52" t="s">
+        <v>62</v>
+      </c>
+      <c r="H52" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I51" s="5" t="s">
+      <c r="I52" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J51" s="9" t="s">
+      <c r="J52" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L51" s="5" t="s">
+      <c r="L52" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M51" s="5" t="s">
+      <c r="M52" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="N51" s="9" t="s">
+      <c r="N52" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H52" s="2" t="s">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="H53" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I52" s="2"/>
-      <c r="L52" s="2" t="s">
+      <c r="I53" s="2"/>
+      <c r="L53" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M52" s="2"/>
-      <c r="N52" s="2"/>
-    </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
-        <v>38</v>
-      </c>
-      <c r="D53" t="s">
-        <v>39</v>
-      </c>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-      <c r="L53" s="2"/>
       <c r="M53" s="2"/>
       <c r="N53" s="2"/>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
+        <v>37</v>
+      </c>
+      <c r="D54" t="s">
         <v>38</v>
       </c>
-      <c r="E54" t="s">
-        <v>66</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L54" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="H54" s="2"/>
+      <c r="I54" s="2"/>
+      <c r="L54" s="2"/>
+      <c r="M54" s="2"/>
+      <c r="N54" s="2"/>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E55" t="s">
-        <v>70</v>
-      </c>
-      <c r="H55" t="s">
-        <v>13</v>
-      </c>
-      <c r="I55" s="1"/>
-      <c r="L55" t="s">
-        <v>13</v>
-      </c>
-      <c r="M55" s="1"/>
-      <c r="N55" s="1"/>
+        <v>65</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L55" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E56" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="H56" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I56" s="1"/>
       <c r="L56" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M56" s="1"/>
       <c r="N56" s="1"/>
     </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.2"/>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B58" t="s">
-        <v>39</v>
-      </c>
-      <c r="E58" t="s">
-        <v>64</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I58" t="s">
-        <v>17</v>
-      </c>
-      <c r="J58" t="s">
-        <v>61</v>
-      </c>
-      <c r="L58" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
+    <row r="57" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
+        <v>37</v>
+      </c>
+      <c r="E57" t="s">
+        <v>62</v>
+      </c>
+      <c r="H57" t="s">
+        <v>14</v>
+      </c>
+      <c r="I57" s="1"/>
+      <c r="L57" t="s">
+        <v>14</v>
+      </c>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+    </row>
+    <row r="58" spans="2:14" x14ac:dyDescent="0.2"/>
     <row r="59" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E59" t="s">
-        <v>65</v>
-      </c>
-      <c r="H59" s="2"/>
-      <c r="L59" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I59" t="s">
+        <v>17</v>
+      </c>
+      <c r="J59" t="s">
+        <v>60</v>
+      </c>
+      <c r="L59" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H60" s="2" t="s">
+      <c r="B60" t="s">
+        <v>38</v>
+      </c>
+      <c r="E60" t="s">
+        <v>64</v>
+      </c>
+      <c r="H60" s="2"/>
+      <c r="L60" s="2"/>
+    </row>
+    <row r="61" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="H61" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I60" s="2"/>
-      <c r="L60" s="2" t="s">
+      <c r="I61" s="2"/>
+      <c r="L61" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M60" s="2"/>
-      <c r="N60" s="2"/>
-    </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B61" t="s">
+      <c r="M61" s="2"/>
+      <c r="N61" s="2"/>
+    </row>
+    <row r="62" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B62" t="s">
         <v>19</v>
       </c>
-      <c r="D61" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="M61" s="1"/>
-      <c r="N61" s="1"/>
-    </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H62" s="2" t="s">
+      <c r="D62" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
+    </row>
+    <row r="63" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="H63" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I62" s="2"/>
-      <c r="L62" s="2" t="s">
+      <c r="I63" s="2"/>
+      <c r="L63" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="M62" s="2"/>
-      <c r="N62" s="2"/>
-    </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="I63" t="s">
-        <v>29</v>
-      </c>
-      <c r="M63" s="15" t="s">
-        <v>28</v>
-      </c>
+      <c r="M63" s="2"/>
+      <c r="N63" s="2"/>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.2">
       <c r="I64" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
     </row>
     <row r="65" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I65" s="15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="66" spans="9:9" x14ac:dyDescent="0.2"/>
+      <c r="I65" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="66" spans="9:9" x14ac:dyDescent="0.2">
+      <c r="I66" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
     <row r="67" spans="9:9" x14ac:dyDescent="0.2"/>
     <row r="68" spans="9:9" x14ac:dyDescent="0.2"/>
     <row r="69" spans="9:9" x14ac:dyDescent="0.2"/>
     <row r="70" spans="9:9" x14ac:dyDescent="0.2"/>
     <row r="71" spans="9:9" x14ac:dyDescent="0.2"/>
-    <row r="72" spans="9:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" spans="9:9" x14ac:dyDescent="0.2"/>
     <row r="73" spans="9:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="74" spans="9:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="75" spans="9:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2434,7 +2532,7 @@
     <row r="84" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="85" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="86" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="93" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="94" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="95" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2443,6 +2541,7 @@
     <row r="98" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="99" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="100" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B4:F4"/>

</xml_diff>

<commit_message>
OO Twenty One - clear_participant_hands, Participant.new_hand
</commit_message>
<xml_diff>
--- a/lesson_5/oo_twenty_one/twenty_one_crc.xlsx
+++ b/lesson_5/oo_twenty_one/twenty_one_crc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswallace/Dropbox/Software-Projects/Launch_School/ls_rb120/lesson_5/oo_twenty_one/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04E90949-677A-D448-ABAE-A2846E7177AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E840041-57D5-3042-A5ED-0794E9A84A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60260" yWindow="-28800" windowWidth="51200" windowHeight="28800" xr2:uid="{49C14D9E-246B-514D-BEB7-B27399C0C8B6}"/>
+    <workbookView xWindow="-60260" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{49C14D9E-246B-514D-BEB7-B27399C0C8B6}"/>
   </bookViews>
   <sheets>
     <sheet name="base_game" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="83">
   <si>
     <t>display_welcome_message</t>
   </si>
@@ -272,6 +272,18 @@
   </si>
   <si>
     <t>Game::TWENTY_ONE_THRESHOLD</t>
+  </si>
+  <si>
+    <t>How to break if participant busts?</t>
+  </si>
+  <si>
+    <t>new_hand</t>
+  </si>
+  <si>
+    <t>clear_participant_hands</t>
+  </si>
+  <si>
+    <t>Participant.new_hand</t>
   </si>
 </sst>
 </file>
@@ -421,7 +433,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2059748</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>106723</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -474,7 +486,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1879600</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>128067</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -527,7 +539,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2062480</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -580,7 +592,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1910080</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -633,7 +645,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2072640</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -686,7 +698,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2113280</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>96051</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -739,7 +751,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2113280</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>64034</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -792,7 +804,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2103120</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>49</xdr:row>
       <xdr:rowOff>132080</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -845,7 +857,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2082800</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -892,13 +904,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1412240</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2082800</xdr:colOff>
-      <xdr:row>64</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -951,7 +963,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2062480</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1004,7 +1016,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>41</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1057,7 +1069,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1104,13 +1116,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1219200</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>117395</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2081092</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>132080</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1157,13 +1169,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1205966</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>117395</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2082800</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>69</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1216,7 +1228,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1896932</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>149412</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1269,7 +1281,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1899663</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>85378</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1322,7 +1334,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1888991</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>128067</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1413,6 +1425,59 @@
         </a:fillRef>
         <a:effectRef idx="0">
           <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1211857</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>85378</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1995714</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>79146</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="123" name="Straight Arrow Connector 122">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7E03FEF-19FB-4045-B9CA-2E4B9642FF3E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6686731" y="4781176"/>
+          <a:ext cx="4903353" cy="4113264"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -1722,11 +1787,9 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E787865A-2D53-2E40-B8D7-C6AC60E2FBBF}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:O101"/>
+  <dimension ref="A1:O105"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="119" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="119" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2007,9 +2070,6 @@
       </c>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C24" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="I24" s="17" t="s">
         <v>70</v>
       </c>
@@ -2019,513 +2079,552 @@
       <c r="M24" s="4"/>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D25" t="s">
+      <c r="C25" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I25" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="L25" s="2"/>
+      <c r="M25" s="4"/>
+    </row>
+    <row r="26" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D26" t="s">
         <v>33</v>
       </c>
-      <c r="H25" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M26" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="I26" s="15" t="s">
+    <row r="27" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="I27" s="15" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="I27" s="16" t="s">
+    <row r="28" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="I28" s="16" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C28" s="2" t="s">
+    <row r="29" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C29" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I28" s="16" t="s">
+      <c r="I29" s="16" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D29" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="30" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D31" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="3:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="D31" t="s">
-        <v>35</v>
-      </c>
-      <c r="H31" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="I31" s="12"/>
-      <c r="J31" s="13"/>
-      <c r="L31" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
     </row>
     <row r="32" spans="3:14" ht="19" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
+        <v>35</v>
+      </c>
+      <c r="H32" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="I32" s="12"/>
+      <c r="J32" s="13"/>
+      <c r="L32" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="M32" s="12"/>
+      <c r="N32" s="12"/>
+    </row>
+    <row r="33" spans="2:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
         <v>18</v>
       </c>
-      <c r="H32" s="6"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="3"/>
-      <c r="N32" s="3"/>
-    </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D33" t="s">
-        <v>9</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I33" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J33" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="L33" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M33" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N33" s="9" t="s">
-        <v>12</v>
-      </c>
+      <c r="H33" s="6"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="L33" s="6"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.2">
       <c r="D34" t="s">
+        <v>9</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J34" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L34" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M34" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N34" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
         <v>1</v>
       </c>
-      <c r="H34" s="2" t="s">
+      <c r="H35" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I34" s="2"/>
-      <c r="L34" s="2" t="s">
+      <c r="I35" s="2"/>
+      <c r="L35" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="L35" s="2"/>
       <c r="M35" s="2"/>
       <c r="N35" s="2"/>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
-        <v>35</v>
-      </c>
-      <c r="D36" t="s">
-        <v>48</v>
-      </c>
-      <c r="E36" t="s">
-        <v>47</v>
-      </c>
-      <c r="F36" t="s">
-        <v>46</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L36" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>35</v>
       </c>
       <c r="D37" t="s">
-        <v>49</v>
-      </c>
-      <c r="H37" t="s">
-        <v>13</v>
-      </c>
-      <c r="I37" s="1"/>
-      <c r="L37" t="s">
-        <v>13</v>
-      </c>
-      <c r="M37" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N37" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="E37" t="s">
+        <v>47</v>
+      </c>
+      <c r="F37" t="s">
+        <v>46</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>35</v>
       </c>
       <c r="D38" t="s">
-        <v>57</v>
-      </c>
-      <c r="H38" t="s">
-        <v>14</v>
-      </c>
-      <c r="I38" s="1"/>
-      <c r="L38" t="s">
-        <v>14</v>
-      </c>
-      <c r="M38" s="1"/>
-      <c r="N38" s="1"/>
+        <v>81</v>
+      </c>
+      <c r="H38" s="2"/>
+      <c r="L38" s="2"/>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>35</v>
       </c>
       <c r="D39" t="s">
-        <v>36</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="H39" t="s">
+        <v>13</v>
+      </c>
+      <c r="I39" s="1"/>
+      <c r="L39" t="s">
+        <v>13</v>
+      </c>
+      <c r="M39" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="N39" s="1"/>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>35</v>
       </c>
       <c r="D40" t="s">
-        <v>37</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I40" t="s">
-        <v>17</v>
-      </c>
-      <c r="J40" t="s">
-        <v>60</v>
-      </c>
-      <c r="L40" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M40" t="s">
-        <v>17</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="H40" t="s">
+        <v>14</v>
+      </c>
+      <c r="I40" s="1"/>
+      <c r="L40" t="s">
+        <v>14</v>
+      </c>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>35</v>
       </c>
       <c r="D41" t="s">
-        <v>19</v>
-      </c>
-      <c r="H41" s="2"/>
-      <c r="L41" s="2"/>
+        <v>36</v>
+      </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>35</v>
+      </c>
+      <c r="D42" t="s">
+        <v>37</v>
+      </c>
       <c r="H42" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I42" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="I42" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42" t="s">
+        <v>60</v>
+      </c>
       <c r="L42" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M42" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="N42" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="M42" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>49</v>
-      </c>
-      <c r="E43" t="s">
-        <v>69</v>
+        <v>35</v>
+      </c>
+      <c r="D43" t="s">
+        <v>19</v>
       </c>
       <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
       <c r="L43" s="2"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="2"/>
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H44" s="2"/>
+      <c r="H44" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="I44" s="2"/>
-      <c r="L44" s="2"/>
-      <c r="M44" s="14"/>
+      <c r="L44" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M44" s="14" t="s">
+        <v>43</v>
+      </c>
       <c r="N44" s="2"/>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E45" t="s">
-        <v>59</v>
-      </c>
-      <c r="I45" s="1"/>
-      <c r="M45" s="1"/>
-      <c r="N45" s="1"/>
+        <v>69</v>
+      </c>
+      <c r="H45" s="2"/>
+      <c r="I45" s="2"/>
+      <c r="L45" s="2"/>
+      <c r="M45" s="14"/>
+      <c r="N45" s="2"/>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
-        <v>57</v>
-      </c>
-      <c r="E46" t="s">
-        <v>63</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>3</v>
-      </c>
+      <c r="H46" s="2"/>
       <c r="I46" s="2"/>
-      <c r="L46" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="14"/>
       <c r="N46" s="2"/>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
+        <v>81</v>
+      </c>
+      <c r="E47" t="s">
+        <v>82</v>
+      </c>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2"/>
+      <c r="L47" s="2"/>
+      <c r="M47" s="14"/>
+      <c r="N47" s="2"/>
+    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="H48" s="2"/>
+      <c r="I48" s="2"/>
+      <c r="L48" s="2"/>
+      <c r="M48" s="14"/>
+      <c r="N48" s="2"/>
+    </row>
+    <row r="49" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B49" t="s">
         <v>57</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E49" t="s">
+        <v>59</v>
+      </c>
+      <c r="I49" s="1"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+    </row>
+    <row r="50" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B50" t="s">
+        <v>57</v>
+      </c>
+      <c r="E50" t="s">
+        <v>63</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I50" s="2"/>
+      <c r="L50" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
+    </row>
+    <row r="51" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B51" t="s">
+        <v>57</v>
+      </c>
+      <c r="E51" t="s">
         <v>64</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I51" t="s">
         <v>34</v>
       </c>
-      <c r="M47" t="s">
+      <c r="M51" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="I48" t="s">
+    <row r="52" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="I52" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.2"/>
-    <row r="50" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="2:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
         <v>36</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E54" t="s">
         <v>61</v>
       </c>
-      <c r="H50" s="12" t="s">
+      <c r="H54" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="I50" s="12"/>
-      <c r="J50" s="13"/>
-      <c r="L50" s="12" t="s">
+      <c r="I54" s="12"/>
+      <c r="J54" s="13"/>
+      <c r="L54" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="M50" s="12"/>
-      <c r="N50" s="12"/>
-    </row>
-    <row r="51" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+      <c r="M54" s="12"/>
+      <c r="N54" s="12"/>
+    </row>
+    <row r="55" spans="2:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
         <v>36</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E55" t="s">
         <v>69</v>
       </c>
-      <c r="H51" s="6"/>
-      <c r="I51" s="3"/>
-      <c r="L51" s="6"/>
-      <c r="M51" s="3"/>
-      <c r="N51" s="3"/>
-    </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B52" t="s">
-        <v>36</v>
-      </c>
-      <c r="E52" t="s">
-        <v>62</v>
-      </c>
-      <c r="H52" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J52" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="L52" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M52" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N52" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H53" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I53" s="2"/>
-      <c r="L53" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="M53" s="2"/>
-      <c r="N53" s="2"/>
-    </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B54" t="s">
-        <v>37</v>
-      </c>
-      <c r="D54" t="s">
-        <v>38</v>
-      </c>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-      <c r="L54" s="2"/>
-      <c r="M54" s="2"/>
-      <c r="N54" s="2"/>
-    </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B55" t="s">
-        <v>37</v>
-      </c>
-      <c r="E55" t="s">
-        <v>65</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L55" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="H55" s="6"/>
+      <c r="I55" s="3"/>
+      <c r="L55" s="6"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="3"/>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
+        <v>36</v>
+      </c>
+      <c r="E56" t="s">
+        <v>62</v>
+      </c>
+      <c r="H56" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I56" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J56" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L56" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="M56" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="N56" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="H57" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I57" s="2"/>
+      <c r="L57" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M57" s="2"/>
+      <c r="N57" s="2"/>
+    </row>
+    <row r="58" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B58" t="s">
         <v>37</v>
       </c>
-      <c r="E56" t="s">
-        <v>69</v>
-      </c>
-      <c r="H56" t="s">
-        <v>13</v>
-      </c>
-      <c r="I56" s="1"/>
-      <c r="L56" t="s">
-        <v>13</v>
-      </c>
-      <c r="M56" s="1"/>
-      <c r="N56" s="1"/>
-    </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
-        <v>37</v>
-      </c>
-      <c r="E57" t="s">
-        <v>62</v>
-      </c>
-      <c r="H57" t="s">
-        <v>14</v>
-      </c>
-      <c r="I57" s="1"/>
-      <c r="L57" t="s">
-        <v>14</v>
-      </c>
-      <c r="M57" s="1"/>
-      <c r="N57" s="1"/>
-    </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.2"/>
+      <c r="D58" t="s">
+        <v>38</v>
+      </c>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+      <c r="L58" s="2"/>
+      <c r="M58" s="2"/>
+      <c r="N58" s="2"/>
+    </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E59" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I59" t="s">
-        <v>17</v>
-      </c>
-      <c r="J59" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="L59" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
+        <v>37</v>
+      </c>
+      <c r="E60" t="s">
+        <v>69</v>
+      </c>
+      <c r="H60" t="s">
+        <v>13</v>
+      </c>
+      <c r="I60" s="1"/>
+      <c r="L60" t="s">
+        <v>13</v>
+      </c>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+    </row>
+    <row r="61" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B61" t="s">
+        <v>37</v>
+      </c>
+      <c r="E61" t="s">
+        <v>62</v>
+      </c>
+      <c r="H61" t="s">
+        <v>14</v>
+      </c>
+      <c r="I61" s="1"/>
+      <c r="L61" t="s">
+        <v>14</v>
+      </c>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+    </row>
+    <row r="62" spans="2:14" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B63" t="s">
         <v>38</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E63" t="s">
+        <v>63</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I63" t="s">
+        <v>17</v>
+      </c>
+      <c r="J63" t="s">
+        <v>60</v>
+      </c>
+      <c r="L63" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="64" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
+        <v>38</v>
+      </c>
+      <c r="E64" t="s">
         <v>64</v>
       </c>
-      <c r="H60" s="2"/>
-      <c r="L60" s="2"/>
-    </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H61" s="2" t="s">
+      <c r="H64" s="2"/>
+      <c r="L64" s="2"/>
+    </row>
+    <row r="65" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="H65" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I61" s="2"/>
-      <c r="L61" s="2" t="s">
+      <c r="I65" s="2"/>
+      <c r="L65" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="M61" s="2"/>
-      <c r="N61" s="2"/>
-    </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B62" t="s">
+      <c r="M65" s="2"/>
+      <c r="N65" s="2"/>
+    </row>
+    <row r="66" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
         <v>19</v>
       </c>
-      <c r="D62" s="16" t="s">
+      <c r="D66" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="M62" s="1"/>
-      <c r="N62" s="1"/>
-    </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H63" s="2" t="s">
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+    </row>
+    <row r="67" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="H67" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I63" s="2"/>
-      <c r="L63" s="2" t="s">
+      <c r="I67" s="2"/>
+      <c r="L67" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="M63" s="2"/>
-      <c r="N63" s="2"/>
-    </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="I64" t="s">
+      <c r="M67" s="2"/>
+      <c r="N67" s="2"/>
+    </row>
+    <row r="68" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="I68" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="65" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I65" t="s">
+    <row r="69" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="I69" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="9:9" x14ac:dyDescent="0.2">
-      <c r="I66" s="15" t="s">
+    <row r="70" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D70" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="I70" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="67" spans="9:9" x14ac:dyDescent="0.2"/>
-    <row r="68" spans="9:9" x14ac:dyDescent="0.2"/>
-    <row r="69" spans="9:9" x14ac:dyDescent="0.2"/>
-    <row r="70" spans="9:9" x14ac:dyDescent="0.2"/>
-    <row r="71" spans="9:9" x14ac:dyDescent="0.2"/>
-    <row r="72" spans="9:9" x14ac:dyDescent="0.2"/>
-    <row r="73" spans="9:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" spans="9:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" spans="9:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" spans="9:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" spans="9:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" spans="9:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" spans="9:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" spans="9:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" spans="2:14" x14ac:dyDescent="0.2"/>
+    <row r="72" spans="2:14" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="2:14" x14ac:dyDescent="0.2"/>
+    <row r="74" spans="2:14" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="2:14" x14ac:dyDescent="0.2"/>
+    <row r="76" spans="2:14" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="2:14" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="2:14" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="2:14" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="2:14" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="81" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="82" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="83" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2533,15 +2632,19 @@
     <row r="85" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="86" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="87" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="97" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="98" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="99" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="100" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="101" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="105" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B4:F4"/>

</xml_diff>

<commit_message>
OO Twenty One - display_hand, deal_card, display_busted, display_winner, participant_busted?
</commit_message>
<xml_diff>
--- a/lesson_5/oo_twenty_one/twenty_one_crc.xlsx
+++ b/lesson_5/oo_twenty_one/twenty_one_crc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswallace/Dropbox/Software-Projects/Launch_School/ls_rb120/lesson_5/oo_twenty_one/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E840041-57D5-3042-A5ED-0794E9A84A99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E32BEE-5527-624B-8788-3B1C008E8454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60260" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{49C14D9E-246B-514D-BEB7-B27399C0C8B6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="93">
   <si>
     <t>display_welcome_message</t>
   </si>
@@ -112,9 +112,6 @@
     <t>Card</t>
   </si>
   <si>
-    <t>Hand (module)</t>
-  </si>
-  <si>
     <t>Participant</t>
   </si>
   <si>
@@ -274,9 +271,6 @@
     <t>Game::TWENTY_ONE_THRESHOLD</t>
   </si>
   <si>
-    <t>How to break if participant busts?</t>
-  </si>
-  <si>
     <t>new_hand</t>
   </si>
   <si>
@@ -284,13 +278,49 @@
   </si>
   <si>
     <t>Participant.new_hand</t>
+  </si>
+  <si>
+    <t>normalize</t>
+  </si>
+  <si>
+    <t>HIT_THRESHOLD</t>
+  </si>
+  <si>
+    <t>receive_card</t>
+  </si>
+  <si>
+    <t>display_card</t>
+  </si>
+  <si>
+    <t>Protected:</t>
+  </si>
+  <si>
+    <t>participant_busted?</t>
+  </si>
+  <si>
+    <t>display_busted</t>
+  </si>
+  <si>
+    <t>display_game_winner</t>
+  </si>
+  <si>
+    <t>display_winner</t>
+  </si>
+  <si>
+    <t>Participant.name</t>
+  </si>
+  <si>
+    <t>Participant.&gt;</t>
+  </si>
+  <si>
+    <t>Participant.==</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -330,19 +360,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -377,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -392,18 +423,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,7 +466,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2059748</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>106723</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -486,7 +519,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1879600</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>128067</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -539,7 +572,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2062480</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -592,7 +625,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1910080</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>45</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -645,7 +678,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2072640</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:row>63</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -698,7 +731,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2113280</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>96051</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -751,7 +784,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2113280</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>64034</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -804,7 +837,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2103120</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>54</xdr:row>
       <xdr:rowOff>132080</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -857,7 +890,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2082800</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -904,13 +937,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1412240</xdr:colOff>
-      <xdr:row>48</xdr:row>
+      <xdr:row>53</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2082800</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -963,7 +996,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2062480</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1016,7 +1049,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>41</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1069,7 +1102,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1116,13 +1149,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1219200</xdr:colOff>
-      <xdr:row>51</xdr:row>
+      <xdr:row>56</xdr:row>
       <xdr:rowOff>117395</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2081092</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>132080</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1169,13 +1202,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1205966</xdr:colOff>
-      <xdr:row>58</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>117395</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2082800</xdr:colOff>
-      <xdr:row>69</xdr:row>
+      <xdr:row>76</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1228,7 +1261,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1896932</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>62</xdr:row>
       <xdr:rowOff>149412</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1281,7 +1314,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1899663</xdr:colOff>
-      <xdr:row>59</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>85378</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1327,15 +1360,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>960504</xdr:colOff>
+      <xdr:colOff>971176</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>96050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1888991</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>128067</xdr:rowOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>138739</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1350,8 +1383,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="6435378" y="4247563"/>
-          <a:ext cx="11312605" cy="3788655"/>
+          <a:off x="6446050" y="4247563"/>
+          <a:ext cx="11301933" cy="4343613"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1436,7 +1469,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1211857</xdr:colOff>
+      <xdr:colOff>1259328</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>85378</xdr:rowOff>
     </xdr:from>
@@ -1444,7 +1477,7 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>1995714</xdr:colOff>
       <xdr:row>46</xdr:row>
-      <xdr:rowOff>79146</xdr:rowOff>
+      <xdr:rowOff>85379</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1459,8 +1492,432 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="6686731" y="4781176"/>
-          <a:ext cx="4903353" cy="4113264"/>
+          <a:off x="6734202" y="4781176"/>
+          <a:ext cx="4855882" cy="3575211"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1195294</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>106723</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2081092</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>138739</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="127" name="Straight Arrow Connector 126">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C326F7B2-4188-B04C-B929-D45A01F92809}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6670168" y="3895378"/>
+          <a:ext cx="5005294" cy="10277395"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1120588</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>117395</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2049075</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>117395</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="130" name="Straight Arrow Connector 129">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD2483DC-1701-4746-891A-02E7A22EFF9C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6595462" y="3906050"/>
+          <a:ext cx="5047983" cy="10608236"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1099244</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>96051</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2123781</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>128068</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="132" name="Straight Arrow Connector 131">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28178466-F22C-2647-B763-7833A54B8297}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6574118" y="2251849"/>
+          <a:ext cx="5144033" cy="12454538"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1035210</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>85378</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2123781</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>96050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="134" name="Straight Arrow Connector 133">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A87BA71-47B0-374B-985F-59B97DC21915}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6510084" y="2241176"/>
+          <a:ext cx="5208067" cy="13158908"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1045882</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>117395</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2113109</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>96051</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="136" name="Straight Arrow Connector 135">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBAC4682-3FE3-B14F-A4AB-642BF7EDF624}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6520756" y="4450336"/>
+          <a:ext cx="5186723" cy="11131177"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1056555</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>138739</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2081092</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>128067</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="138" name="Straight Arrow Connector 137">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1043593A-3013-054F-96E5-E99F87AFA453}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6531429" y="4653109"/>
+          <a:ext cx="5144033" cy="11141849"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1045882</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>85378</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2123781</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>117395</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="145" name="Straight Arrow Connector 144">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B651C42-C7F2-664D-BD88-1C14E6FE6D13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6520756" y="2241176"/>
+          <a:ext cx="5197395" cy="9423614"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>992521</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>74706</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2113109</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>117395</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="147" name="Straight Arrow Connector 146">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2BBCCB0A-A687-D04E-86D1-A6FC5C140264}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="6467395" y="2230504"/>
+          <a:ext cx="5240084" cy="10469496"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1787,9 +2244,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E787865A-2D53-2E40-B8D7-C6AC60E2FBBF}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:O105"/>
+  <dimension ref="A1:O117"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="119" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="119" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1814,25 +2273,25 @@
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.2"/>
     <row r="4" spans="2:15" ht="22" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
+      <c r="H4" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="18"/>
+      <c r="J4" s="18"/>
       <c r="K4" s="3"/>
-      <c r="L4" s="12" t="s">
+      <c r="L4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
       <c r="O4" s="3"/>
     </row>
     <row r="5" spans="2:15" ht="22" customHeight="1" x14ac:dyDescent="0.25">
@@ -1857,10 +2316,10 @@
       <c r="D6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="10"/>
+      <c r="F6" s="19"/>
       <c r="G6" s="3"/>
       <c r="H6" s="5" t="s">
         <v>10</v>
@@ -1894,21 +2353,21 @@
         <v>5</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="N7" s="2"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">
       <c r="M9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.2">
@@ -1931,13 +2390,13 @@
         <v>13</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L11" t="s">
         <v>13</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N11" s="1"/>
     </row>
@@ -1950,13 +2409,13 @@
         <v>14</v>
       </c>
       <c r="I12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="L12" t="s">
         <v>14</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N12" s="1"/>
     </row>
@@ -1990,7 +2449,7 @@
         <v>4</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>4</v>
@@ -2000,28 +2459,28 @@
     </row>
     <row r="17" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E17" t="s">
         <v>7</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N17" s="1"/>
     </row>
     <row r="18" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E18" t="s">
         <v>30</v>
       </c>
-      <c r="E18" t="s">
-        <v>31</v>
-      </c>
       <c r="I18" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.2">
@@ -2036,11 +2495,11 @@
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.2">
       <c r="H20" s="4"/>
-      <c r="I20" s="16" t="s">
-        <v>27</v>
+      <c r="I20" s="14" t="s">
+        <v>26</v>
       </c>
       <c r="J20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M20" t="s">
         <v>6</v>
@@ -2048,30 +2507,30 @@
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.2">
       <c r="I21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="M21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.2">
       <c r="I22" t="s">
-        <v>58</v>
-      </c>
-      <c r="M22" s="16" t="s">
-        <v>28</v>
+        <v>57</v>
+      </c>
+      <c r="M22" s="14" t="s">
+        <v>27</v>
       </c>
       <c r="N22" s="4"/>
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D23" s="1"/>
-      <c r="I23" s="16" t="s">
-        <v>68</v>
+      <c r="I23" s="14" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="I24" s="17" t="s">
-        <v>70</v>
+      <c r="I24" s="15" t="s">
+        <v>69</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>2</v>
@@ -2079,563 +2538,582 @@
       <c r="M24" s="4"/>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C25" s="2" t="s">
+      <c r="I25" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="L25" s="2"/>
+      <c r="M25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C26" s="2"/>
+      <c r="I26" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="L26" s="2"/>
+      <c r="M26" s="4"/>
+    </row>
+    <row r="27" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C27" s="2"/>
+      <c r="I27" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="L27" s="2"/>
+      <c r="M27" s="4"/>
+    </row>
+    <row r="28" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C28" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I25" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="L25" s="2"/>
-      <c r="M25" s="4"/>
-    </row>
-    <row r="26" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D26" t="s">
-        <v>33</v>
-      </c>
-      <c r="H26" s="2" t="s">
+      <c r="I28" s="15"/>
+      <c r="L28" s="2"/>
+      <c r="M28" s="4"/>
+    </row>
+    <row r="29" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D29" t="s">
+        <v>32</v>
+      </c>
+      <c r="H29" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="M26" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="I27" s="15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="I28" s="16" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="C29" s="2" t="s">
+    </row>
+    <row r="30" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="H30" s="2"/>
+      <c r="I30" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="I31" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="I32" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="I33" s="14"/>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="H34" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="I34" s="14"/>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C35" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="I29" s="16" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D30" t="s">
+      <c r="I35" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="D31" t="s">
+    <row r="37" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D37" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="3:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="D32" t="s">
-        <v>35</v>
-      </c>
-      <c r="H32" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="I32" s="12"/>
-      <c r="J32" s="13"/>
-      <c r="L32" s="12" t="s">
+    <row r="38" spans="2:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>34</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I38" s="10"/>
+      <c r="J38" s="12"/>
+      <c r="L38" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="M32" s="12"/>
-      <c r="N32" s="12"/>
-    </row>
-    <row r="33" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="D33" t="s">
+      <c r="M38" s="10"/>
+      <c r="N38" s="10"/>
+    </row>
+    <row r="39" spans="2:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>86</v>
+      </c>
+      <c r="H39" s="11"/>
+      <c r="I39" s="11"/>
+      <c r="J39" s="16"/>
+      <c r="L39" s="11"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="11"/>
+    </row>
+    <row r="40" spans="2:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>87</v>
+      </c>
+      <c r="H40" s="11"/>
+      <c r="I40" s="11"/>
+      <c r="J40" s="16"/>
+      <c r="L40" s="11"/>
+      <c r="M40" s="11"/>
+      <c r="N40" s="11"/>
+    </row>
+    <row r="41" spans="2:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>88</v>
+      </c>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="16"/>
+      <c r="L41" s="11"/>
+      <c r="M41" s="11"/>
+      <c r="N41" s="11"/>
+    </row>
+    <row r="42" spans="2:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
         <v>18</v>
       </c>
-      <c r="H33" s="6"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="L33" s="6"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D34" t="s">
+      <c r="H42" s="6"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="L42" s="6"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D43" t="s">
         <v>9</v>
       </c>
-      <c r="H34" s="5" t="s">
+      <c r="H43" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I34" s="5" t="s">
+      <c r="I43" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J34" s="9" t="s">
+      <c r="J43" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L34" s="5" t="s">
+      <c r="L43" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M34" s="5" t="s">
+      <c r="M43" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="N34" s="9" t="s">
+      <c r="N43" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D35" t="s">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D44" t="s">
         <v>1</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="H44" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="I35" s="2"/>
-      <c r="L35" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-    </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-    </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
-        <v>35</v>
-      </c>
-      <c r="D37" t="s">
-        <v>48</v>
-      </c>
-      <c r="E37" t="s">
-        <v>47</v>
-      </c>
-      <c r="F37" t="s">
-        <v>46</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L37" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
-        <v>35</v>
-      </c>
-      <c r="D38" t="s">
-        <v>81</v>
-      </c>
-      <c r="H38" s="2"/>
-      <c r="L38" s="2"/>
-    </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
-        <v>35</v>
-      </c>
-      <c r="D39" t="s">
-        <v>49</v>
-      </c>
-      <c r="H39" t="s">
-        <v>13</v>
-      </c>
-      <c r="I39" s="1"/>
-      <c r="L39" t="s">
-        <v>13</v>
-      </c>
-      <c r="M39" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="N39" s="1"/>
-    </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
-        <v>35</v>
-      </c>
-      <c r="D40" t="s">
-        <v>57</v>
-      </c>
-      <c r="H40" t="s">
-        <v>14</v>
-      </c>
-      <c r="I40" s="1"/>
-      <c r="L40" t="s">
-        <v>14</v>
-      </c>
-      <c r="M40" s="1"/>
-      <c r="N40" s="1"/>
-    </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
-        <v>35</v>
-      </c>
-      <c r="D41" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
-        <v>35</v>
-      </c>
-      <c r="D42" t="s">
-        <v>37</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I42" t="s">
-        <v>17</v>
-      </c>
-      <c r="J42" t="s">
-        <v>60</v>
-      </c>
-      <c r="L42" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M42" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
-        <v>35</v>
-      </c>
-      <c r="D43" t="s">
-        <v>19</v>
-      </c>
-      <c r="H43" s="2"/>
-      <c r="L43" s="2"/>
-    </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H44" s="2" t="s">
-        <v>4</v>
       </c>
       <c r="I44" s="2"/>
       <c r="L44" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M44" s="14" t="s">
-        <v>43</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="M44" s="2"/>
       <c r="N44" s="2"/>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
-        <v>49</v>
-      </c>
-      <c r="E45" t="s">
-        <v>69</v>
-      </c>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
       <c r="L45" s="2"/>
-      <c r="M45" s="14"/>
+      <c r="M45" s="2"/>
       <c r="N45" s="2"/>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="14"/>
-      <c r="N46" s="2"/>
+      <c r="B46" t="s">
+        <v>34</v>
+      </c>
+      <c r="D46" t="s">
+        <v>47</v>
+      </c>
+      <c r="E46" t="s">
+        <v>46</v>
+      </c>
+      <c r="F46" t="s">
+        <v>45</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>81</v>
+        <v>34</v>
+      </c>
+      <c r="D47" t="s">
+        <v>79</v>
       </c>
       <c r="E47" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
       <c r="L47" s="2"/>
-      <c r="M47" s="14"/>
-      <c r="N47" s="2"/>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H48" s="2"/>
-      <c r="I48" s="2"/>
-      <c r="L48" s="2"/>
-      <c r="M48" s="14"/>
-      <c r="N48" s="2"/>
+      <c r="B48" t="s">
+        <v>34</v>
+      </c>
+      <c r="D48" t="s">
+        <v>48</v>
+      </c>
+      <c r="E48" t="s">
+        <v>68</v>
+      </c>
+      <c r="H48" t="s">
+        <v>13</v>
+      </c>
+      <c r="I48" s="1"/>
+      <c r="L48" t="s">
+        <v>13</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N48" s="1"/>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
-        <v>57</v>
-      </c>
-      <c r="E49" t="s">
-        <v>59</v>
+        <v>34</v>
+      </c>
+      <c r="D49" t="s">
+        <v>56</v>
+      </c>
+      <c r="H49" t="s">
+        <v>14</v>
       </c>
       <c r="I49" s="1"/>
+      <c r="L49" t="s">
+        <v>14</v>
+      </c>
       <c r="M49" s="1"/>
       <c r="N49" s="1"/>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>57</v>
-      </c>
-      <c r="E50" t="s">
-        <v>63</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I50" s="2"/>
-      <c r="L50" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M50" s="2"/>
-      <c r="N50" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="D50" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>57</v>
-      </c>
-      <c r="E51" t="s">
-        <v>64</v>
+        <v>34</v>
+      </c>
+      <c r="D51" t="s">
+        <v>36</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="I51" t="s">
-        <v>34</v>
+        <v>17</v>
+      </c>
+      <c r="J51" t="s">
+        <v>59</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="M51" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="I52" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.2"/>
-    <row r="54" spans="2:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>19</v>
+      </c>
+      <c r="H52" s="2"/>
+      <c r="L52" s="2"/>
+    </row>
+    <row r="53" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="H53" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I53" s="2"/>
+      <c r="L53" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M53" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="N53" s="2"/>
+    </row>
+    <row r="54" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="E54" t="s">
-        <v>61</v>
-      </c>
-      <c r="H54" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="I54" s="12"/>
-      <c r="J54" s="13"/>
-      <c r="L54" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="M54" s="12"/>
-      <c r="N54" s="12"/>
-    </row>
-    <row r="55" spans="2:14" ht="19" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="I54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+    </row>
+    <row r="55" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="E55" t="s">
-        <v>69</v>
-      </c>
-      <c r="H55" s="6"/>
-      <c r="I55" s="3"/>
-      <c r="L55" s="6"/>
-      <c r="M55" s="3"/>
-      <c r="N55" s="3"/>
+        <v>62</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I55" s="2"/>
+      <c r="L55" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M55" s="2"/>
+      <c r="N55" s="2"/>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>36</v>
+        <v>56</v>
       </c>
       <c r="E56" t="s">
-        <v>62</v>
-      </c>
-      <c r="H56" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I56" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J56" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="L56" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="M56" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N56" s="9" t="s">
-        <v>12</v>
+        <v>63</v>
+      </c>
+      <c r="I56" t="s">
+        <v>33</v>
+      </c>
+      <c r="M56" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H57" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I57" s="2"/>
-      <c r="L57" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="M57" s="2"/>
-      <c r="N57" s="2"/>
-    </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B58" t="s">
-        <v>37</v>
-      </c>
-      <c r="D58" t="s">
+      <c r="I57" t="s">
         <v>38</v>
       </c>
-      <c r="H58" s="2"/>
-      <c r="I58" s="2"/>
-      <c r="L58" s="2"/>
-      <c r="M58" s="2"/>
-      <c r="N58" s="2"/>
-    </row>
+    </row>
+    <row r="58" spans="2:14" x14ac:dyDescent="0.2"/>
     <row r="59" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B59" t="s">
-        <v>37</v>
-      </c>
-      <c r="E59" t="s">
-        <v>65</v>
-      </c>
       <c r="H59" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L59" s="2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B60" t="s">
-        <v>37</v>
-      </c>
-      <c r="E60" t="s">
-        <v>69</v>
-      </c>
-      <c r="H60" t="s">
-        <v>13</v>
-      </c>
-      <c r="I60" s="1"/>
-      <c r="L60" t="s">
-        <v>13</v>
-      </c>
-      <c r="M60" s="1"/>
-      <c r="N60" s="1"/>
+      <c r="H60" s="2"/>
+      <c r="I60" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E61" t="s">
-        <v>62</v>
-      </c>
-      <c r="H61" t="s">
-        <v>14</v>
-      </c>
-      <c r="I61" s="1"/>
-      <c r="L61" t="s">
-        <v>14</v>
-      </c>
-      <c r="M61" s="1"/>
-      <c r="N61" s="1"/>
-    </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.2"/>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="62" spans="2:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>35</v>
+      </c>
+      <c r="E62" t="s">
+        <v>60</v>
+      </c>
+      <c r="H62" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I62" s="10"/>
+      <c r="J62" s="12"/>
+    </row>
+    <row r="63" spans="2:14" ht="19" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E63" t="s">
-        <v>63</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I63" t="s">
-        <v>17</v>
-      </c>
-      <c r="J63" t="s">
-        <v>60</v>
-      </c>
-      <c r="L63" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="H63" s="6"/>
+      <c r="I63" s="3"/>
     </row>
     <row r="64" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
+        <v>35</v>
+      </c>
+      <c r="E64" t="s">
+        <v>61</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I64" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J64" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H65" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I65" s="2"/>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B66" t="s">
+        <v>36</v>
+      </c>
+      <c r="E66" t="s">
+        <v>90</v>
+      </c>
+      <c r="H66" s="2"/>
+      <c r="I66" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B67" t="s">
+        <v>36</v>
+      </c>
+      <c r="E67" t="s">
+        <v>64</v>
+      </c>
+      <c r="H67" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B68" t="s">
+        <v>36</v>
+      </c>
+      <c r="E68" t="s">
+        <v>68</v>
+      </c>
+      <c r="H68" t="s">
+        <v>13</v>
+      </c>
+      <c r="I68" s="1"/>
+    </row>
+    <row r="69" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B69" t="s">
+        <v>36</v>
+      </c>
+      <c r="E69" t="s">
+        <v>61</v>
+      </c>
+      <c r="H69" t="s">
+        <v>14</v>
+      </c>
+      <c r="I69" s="1"/>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.2"/>
+    <row r="71" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B71" t="s">
+        <v>37</v>
+      </c>
+      <c r="E71" t="s">
+        <v>62</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I71" t="s">
+        <v>17</v>
+      </c>
+      <c r="J71" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B72" t="s">
+        <v>37</v>
+      </c>
+      <c r="E72" t="s">
+        <v>63</v>
+      </c>
+      <c r="H72" s="2"/>
+    </row>
+    <row r="73" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H73" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I73" s="2"/>
+    </row>
+    <row r="74" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B74" t="s">
+        <v>86</v>
+      </c>
+      <c r="E74" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="75" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H75" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I75" s="2"/>
+    </row>
+    <row r="76" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B76" t="s">
+        <v>87</v>
+      </c>
+      <c r="E76" t="s">
+        <v>61</v>
+      </c>
+      <c r="I76" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="77" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="E77" t="s">
+        <v>90</v>
+      </c>
+      <c r="I77" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="E64" t="s">
-        <v>64</v>
-      </c>
-      <c r="H64" s="2"/>
-      <c r="L64" s="2"/>
-    </row>
-    <row r="65" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H65" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I65" s="2"/>
-      <c r="L65" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M65" s="2"/>
-      <c r="N65" s="2"/>
-    </row>
-    <row r="66" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B66" t="s">
-        <v>19</v>
-      </c>
-      <c r="D66" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="M66" s="1"/>
-      <c r="N66" s="1"/>
-    </row>
-    <row r="67" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H67" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I67" s="2"/>
-      <c r="L67" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M67" s="2"/>
-      <c r="N67" s="2"/>
-    </row>
-    <row r="68" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="I68" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="69" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="I69" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="70" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D70" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="I70" s="16" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="71" spans="2:14" x14ac:dyDescent="0.2"/>
-    <row r="72" spans="2:14" x14ac:dyDescent="0.2"/>
-    <row r="73" spans="2:14" x14ac:dyDescent="0.2"/>
-    <row r="74" spans="2:14" x14ac:dyDescent="0.2"/>
-    <row r="75" spans="2:14" x14ac:dyDescent="0.2"/>
-    <row r="76" spans="2:14" x14ac:dyDescent="0.2"/>
-    <row r="77" spans="2:14" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" spans="2:14" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" spans="2:14" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" spans="2:14" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="78" spans="2:10" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B79" t="s">
+        <v>89</v>
+      </c>
+      <c r="D79" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10" x14ac:dyDescent="0.2"/>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B81" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E81" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E82" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="E83" s="17" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="97" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="98" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="99" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2645,6 +3123,18 @@
     <row r="103" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="104" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="105" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="106" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="107" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="108" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="109" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="110" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="113" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="117" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B4:F4"/>

</xml_diff>

<commit_message>
OO Twenty One - refactor accessors and keyword argument for deal_initial_cards (for Rubocop)
</commit_message>
<xml_diff>
--- a/lesson_5/oo_twenty_one/twenty_one_crc.xlsx
+++ b/lesson_5/oo_twenty_one/twenty_one_crc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswallace/Dropbox/Software-Projects/Launch_School/ls_rb120/lesson_5/oo_twenty_one/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E32BEE-5527-624B-8788-3B1C008E8454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEA60DF-E032-FA43-95E5-95F47A48E57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60260" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{49C14D9E-246B-514D-BEB7-B27399C0C8B6}"/>
+    <workbookView xWindow="-60260" yWindow="-28800" windowWidth="51200" windowHeight="28800" xr2:uid="{49C14D9E-246B-514D-BEB7-B27399C0C8B6}"/>
   </bookViews>
   <sheets>
     <sheet name="base_game" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="91">
   <si>
     <t>display_welcome_message</t>
   </si>
@@ -154,9 +154,6 @@
     <t>choose_move</t>
   </si>
   <si>
-    <t>deck</t>
-  </si>
-  <si>
     <t>@deck</t>
   </si>
   <si>
@@ -253,12 +250,6 @@
     <t>@hand</t>
   </si>
   <si>
-    <t>hand_values</t>
-  </si>
-  <si>
-    <t>name, hand, hand_values</t>
-  </si>
-  <si>
     <t>@hand_values</t>
   </si>
   <si>
@@ -314,6 +305,9 @@
   </si>
   <si>
     <t>Participant.==</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -1072,7 +1066,8 @@
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
-          <a:tailEnd type="triangle"/>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="none"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -1125,7 +1120,8 @@
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
-          <a:tailEnd type="triangle"/>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="none"/>
         </a:ln>
       </xdr:spPr>
       <xdr:style>
@@ -2247,7 +2243,7 @@
   <dimension ref="A1:O117"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -2353,21 +2349,21 @@
         <v>5</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N7" s="2"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="M8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">
       <c r="M9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.2">
@@ -2390,14 +2386,12 @@
         <v>13</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="L11" t="s">
         <v>13</v>
       </c>
-      <c r="M11" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="M11" s="1"/>
       <c r="N11" s="1"/>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.2">
@@ -2408,15 +2402,10 @@
       <c r="H12" t="s">
         <v>14</v>
       </c>
-      <c r="I12" t="s">
-        <v>72</v>
-      </c>
       <c r="L12" t="s">
         <v>14</v>
       </c>
-      <c r="M12" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="M12" s="1"/>
       <c r="N12" s="1"/>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.2"/>
@@ -2465,10 +2454,10 @@
         <v>7</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N17" s="1"/>
     </row>
@@ -2480,7 +2469,7 @@
         <v>30</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.2">
@@ -2499,7 +2488,7 @@
         <v>26</v>
       </c>
       <c r="J20" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="M20" t="s">
         <v>6</v>
@@ -2507,15 +2496,15 @@
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.2">
       <c r="I21" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="M21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.2">
       <c r="I22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M22" s="14" t="s">
         <v>27</v>
@@ -2525,12 +2514,12 @@
     <row r="23" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D23" s="1"/>
       <c r="I23" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.2">
       <c r="I24" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>2</v>
@@ -2539,17 +2528,17 @@
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.2">
       <c r="I25" s="15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="L25" s="2"/>
       <c r="M25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C26" s="2"/>
       <c r="I26" s="15" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="L26" s="2"/>
       <c r="M26" s="4"/>
@@ -2557,7 +2546,7 @@
     <row r="27" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C27" s="2"/>
       <c r="I27" s="15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="L27" s="2"/>
       <c r="M27" s="4"/>
@@ -2586,12 +2575,12 @@
     </row>
     <row r="31" spans="3:14" x14ac:dyDescent="0.2">
       <c r="I31" s="14" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="3:14" x14ac:dyDescent="0.2">
       <c r="I32" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="2:14" x14ac:dyDescent="0.2">
@@ -2599,7 +2588,7 @@
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.2">
       <c r="H34" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="I34" s="14"/>
     </row>
@@ -2608,7 +2597,7 @@
         <v>2</v>
       </c>
       <c r="I35" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.2">
@@ -2626,7 +2615,7 @@
         <v>34</v>
       </c>
       <c r="H38" s="10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="I38" s="10"/>
       <c r="J38" s="12"/>
@@ -2638,7 +2627,7 @@
     </row>
     <row r="39" spans="2:14" ht="19" x14ac:dyDescent="0.25">
       <c r="D39" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H39" s="11"/>
       <c r="I39" s="11"/>
@@ -2649,7 +2638,7 @@
     </row>
     <row r="40" spans="2:14" ht="19" x14ac:dyDescent="0.25">
       <c r="D40" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H40" s="11"/>
       <c r="I40" s="11"/>
@@ -2660,7 +2649,7 @@
     </row>
     <row r="41" spans="2:14" ht="19" x14ac:dyDescent="0.25">
       <c r="D41" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="H41" s="11"/>
       <c r="I41" s="11"/>
@@ -2729,13 +2718,13 @@
         <v>34</v>
       </c>
       <c r="D46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E46" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F46" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>15</v>
@@ -2749,10 +2738,10 @@
         <v>34</v>
       </c>
       <c r="D47" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E47" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H47" s="2"/>
       <c r="L47" s="2"/>
@@ -2762,10 +2751,10 @@
         <v>34</v>
       </c>
       <c r="D48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H48" t="s">
         <v>13</v>
@@ -2775,7 +2764,7 @@
         <v>13</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N48" s="1"/>
     </row>
@@ -2784,7 +2773,7 @@
         <v>34</v>
       </c>
       <c r="D49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H49" t="s">
         <v>14</v>
@@ -2818,7 +2807,7 @@
         <v>17</v>
       </c>
       <c r="J51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L51" s="2" t="s">
         <v>16</v>
@@ -2843,16 +2832,16 @@
         <v>4</v>
       </c>
       <c r="M53" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="N53" s="2"/>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I54" s="1"/>
       <c r="M54" s="1"/>
@@ -2860,10 +2849,10 @@
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E55" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H55" s="2" t="s">
         <v>3</v>
@@ -2877,10 +2866,10 @@
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E56" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I56" t="s">
         <v>33</v>
@@ -2903,7 +2892,7 @@
     <row r="60" spans="2:14" x14ac:dyDescent="0.2">
       <c r="H60" s="2"/>
       <c r="I60" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.2">
@@ -2911,7 +2900,7 @@
         <v>35</v>
       </c>
       <c r="E61" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="62" spans="2:14" ht="19" x14ac:dyDescent="0.25">
@@ -2919,10 +2908,10 @@
         <v>35</v>
       </c>
       <c r="E62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H62" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="I62" s="10"/>
       <c r="J62" s="12"/>
@@ -2932,7 +2921,7 @@
         <v>35</v>
       </c>
       <c r="E63" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H63" s="6"/>
       <c r="I63" s="3"/>
@@ -2942,7 +2931,7 @@
         <v>35</v>
       </c>
       <c r="E64" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H64" s="5" t="s">
         <v>10</v>
@@ -2965,11 +2954,11 @@
         <v>36</v>
       </c>
       <c r="E66" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H66" s="2"/>
       <c r="I66" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="67" spans="2:10" x14ac:dyDescent="0.2">
@@ -2977,7 +2966,7 @@
         <v>36</v>
       </c>
       <c r="E67" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H67" s="2" t="s">
         <v>15</v>
@@ -2988,7 +2977,7 @@
         <v>36</v>
       </c>
       <c r="E68" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H68" t="s">
         <v>13</v>
@@ -3000,7 +2989,7 @@
         <v>36</v>
       </c>
       <c r="E69" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H69" t="s">
         <v>14</v>
@@ -3013,7 +3002,7 @@
         <v>37</v>
       </c>
       <c r="E71" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H71" s="2" t="s">
         <v>16</v>
@@ -3022,7 +3011,7 @@
         <v>17</v>
       </c>
       <c r="J71" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.2">
@@ -3030,7 +3019,7 @@
         <v>37</v>
       </c>
       <c r="E72" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H72" s="2"/>
     </row>
@@ -3042,10 +3031,10 @@
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E74" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="75" spans="2:10" x14ac:dyDescent="0.2">
@@ -3056,18 +3045,18 @@
     </row>
     <row r="76" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E76" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I76" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.2">
       <c r="E77" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I77" s="14" t="s">
         <v>38</v>
@@ -3076,29 +3065,29 @@
     <row r="78" spans="2:10" x14ac:dyDescent="0.2"/>
     <row r="79" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D79" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="80" spans="2:10" x14ac:dyDescent="0.2"/>
     <row r="81" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B81" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E81" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="82" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E82" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="83" spans="2:5" x14ac:dyDescent="0.2">
       <c r="E83" s="17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="84" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
OO Twenty One - account for ace value permutations
</commit_message>
<xml_diff>
--- a/lesson_5/oo_twenty_one/twenty_one_crc.xlsx
+++ b/lesson_5/oo_twenty_one/twenty_one_crc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswallace/Dropbox/Software-Projects/Launch_School/ls_rb120/lesson_5/oo_twenty_one/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEA60DF-E032-FA43-95E5-95F47A48E57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502A54B8-74D4-A144-A757-6E6C0484B691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60260" yWindow="-28800" windowWidth="51200" windowHeight="28800" xr2:uid="{49C14D9E-246B-514D-BEB7-B27399C0C8B6}"/>
+    <workbookView xWindow="-60260" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{49C14D9E-246B-514D-BEB7-B27399C0C8B6}"/>
   </bookViews>
   <sheets>
     <sheet name="base_game" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="98">
   <si>
     <t>display_welcome_message</t>
   </si>
@@ -148,9 +148,6 @@
     <t>dealer_turn</t>
   </si>
   <si>
-    <t>display_participant_cards</t>
-  </si>
-  <si>
     <t>choose_move</t>
   </si>
   <si>
@@ -205,9 +202,6 @@
     <t>display_hands_for_player</t>
   </si>
   <si>
-    <t>display_hand_value</t>
-  </si>
-  <si>
     <t>Dealer.display_first_card</t>
   </si>
   <si>
@@ -223,9 +217,6 @@
     <t>Participant.display_hand</t>
   </si>
   <si>
-    <t>Participant.display_hand_value</t>
-  </si>
-  <si>
     <t>Dealer.choose_move</t>
   </si>
   <si>
@@ -308,6 +299,36 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>display_final_participant_cards</t>
+  </si>
+  <si>
+    <t>Participant.display_max_hand_value</t>
+  </si>
+  <si>
+    <t>display_max_hand_value</t>
+  </si>
+  <si>
+    <t>Participant.display_hand_values</t>
+  </si>
+  <si>
+    <t>display_hand_values</t>
+  </si>
+  <si>
+    <t>values_below_threshold</t>
+  </si>
+  <si>
+    <t>joiner</t>
+  </si>
+  <si>
+    <t>sum_non_aves</t>
+  </si>
+  <si>
+    <t>possible_ace_values</t>
+  </si>
+  <si>
+    <t>possible_hand_values</t>
   </si>
 </sst>
 </file>
@@ -460,7 +481,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2059748</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>106723</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -513,7 +534,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1879600</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>128067</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -566,7 +587,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2062480</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -619,7 +640,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1910080</xdr:colOff>
-      <xdr:row>45</xdr:row>
+      <xdr:row>50</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -672,7 +693,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2072640</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>68</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -725,7 +746,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2113280</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>96051</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -772,13 +793,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1675546</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>106723</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2113280</xdr:colOff>
-      <xdr:row>71</xdr:row>
+      <xdr:colOff>2091764</xdr:colOff>
+      <xdr:row>76</xdr:row>
       <xdr:rowOff>64034</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -794,8 +815,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="7150420" y="4303913"/>
-          <a:ext cx="4557230" cy="6517768"/>
+          <a:off x="7150420" y="4439664"/>
+          <a:ext cx="4535714" cy="9295546"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -831,7 +852,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2103120</xdr:colOff>
-      <xdr:row>54</xdr:row>
+      <xdr:row>59</xdr:row>
       <xdr:rowOff>132080</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -879,12 +900,12 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>1778000</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>172720</xdr:rowOff>
+      <xdr:rowOff>117395</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2082800</xdr:colOff>
-      <xdr:row>55</xdr:row>
+      <xdr:colOff>2123781</xdr:colOff>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -900,8 +921,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="7264400" y="4368800"/>
-          <a:ext cx="4439920" cy="4074160"/>
+          <a:off x="7252874" y="4268908"/>
+          <a:ext cx="4465277" cy="6472944"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -931,13 +952,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1412240</xdr:colOff>
-      <xdr:row>53</xdr:row>
+      <xdr:row>58</xdr:row>
       <xdr:rowOff>121920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2082800</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -990,7 +1011,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2062480</xdr:colOff>
-      <xdr:row>68</xdr:row>
+      <xdr:row>73</xdr:row>
       <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1043,7 +1064,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>50</xdr:row>
+      <xdr:row>55</xdr:row>
       <xdr:rowOff>60960</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1097,7 +1118,7 @@
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>70</xdr:row>
+      <xdr:row>75</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1145,13 +1166,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1219200</xdr:colOff>
-      <xdr:row>56</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>117395</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2081092</xdr:colOff>
-      <xdr:row>61</xdr:row>
+      <xdr:row>66</xdr:row>
       <xdr:rowOff>132080</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1198,13 +1219,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1205966</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>71</xdr:row>
       <xdr:rowOff>117395</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2082800</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1257,7 +1278,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1896932</xdr:colOff>
-      <xdr:row>62</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>149412</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1310,7 +1331,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1899663</xdr:colOff>
-      <xdr:row>67</xdr:row>
+      <xdr:row>72</xdr:row>
       <xdr:rowOff>85378</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1363,7 +1384,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>1888991</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>52</xdr:row>
       <xdr:rowOff>138739</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1466,13 +1487,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1259328</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>85378</xdr:rowOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>138739</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>1995714</xdr:colOff>
-      <xdr:row>46</xdr:row>
+      <xdr:colOff>2070420</xdr:colOff>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>85379</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1488,8 +1509,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="6734202" y="4781176"/>
-          <a:ext cx="4855882" cy="3575211"/>
+          <a:off x="6734202" y="5015966"/>
+          <a:ext cx="4930588" cy="4076808"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1525,7 +1546,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2081092</xdr:colOff>
-      <xdr:row>73</xdr:row>
+      <xdr:row>78</xdr:row>
       <xdr:rowOff>138739</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1578,7 +1599,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2049075</xdr:colOff>
-      <xdr:row>75</xdr:row>
+      <xdr:row>80</xdr:row>
       <xdr:rowOff>117395</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1631,7 +1652,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2123781</xdr:colOff>
-      <xdr:row>76</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>128068</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1684,7 +1705,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2123781</xdr:colOff>
-      <xdr:row>80</xdr:row>
+      <xdr:row>85</xdr:row>
       <xdr:rowOff>96050</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1731,13 +1752,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1045882</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>117395</xdr:rowOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>128067</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2113109</xdr:colOff>
-      <xdr:row>81</xdr:row>
+      <xdr:colOff>2091764</xdr:colOff>
+      <xdr:row>86</xdr:row>
       <xdr:rowOff>96051</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1753,8 +1774,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="6520756" y="4450336"/>
-          <a:ext cx="5186723" cy="11131177"/>
+          <a:off x="6520756" y="4642437"/>
+          <a:ext cx="5165378" cy="10939076"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1784,13 +1805,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>1056555</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>138739</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>128068</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>2081092</xdr:colOff>
-      <xdr:row>82</xdr:row>
+      <xdr:colOff>2113109</xdr:colOff>
+      <xdr:row>87</xdr:row>
       <xdr:rowOff>128067</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1806,8 +1827,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="6531429" y="4653109"/>
-          <a:ext cx="5144033" cy="11141849"/>
+          <a:off x="6531429" y="4823866"/>
+          <a:ext cx="5176050" cy="10971092"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1843,7 +1864,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2123781</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>65</xdr:row>
       <xdr:rowOff>117395</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1896,7 +1917,7 @@
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>2113109</xdr:colOff>
-      <xdr:row>65</xdr:row>
+      <xdr:row>70</xdr:row>
       <xdr:rowOff>117395</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2240,10 +2261,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E787865A-2D53-2E40-B8D7-C6AC60E2FBBF}">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A1:O117"/>
+  <dimension ref="A1:O122"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="E36" sqref="E36:E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -2349,21 +2370,21 @@
         <v>5</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="N7" s="2"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="M8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.2">
       <c r="M9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.2">
@@ -2386,7 +2407,7 @@
         <v>13</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="L11" t="s">
         <v>13</v>
@@ -2454,10 +2475,10 @@
         <v>7</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N17" s="1"/>
     </row>
@@ -2469,7 +2490,7 @@
         <v>30</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.2">
@@ -2488,7 +2509,7 @@
         <v>26</v>
       </c>
       <c r="J20" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="M20" t="s">
         <v>6</v>
@@ -2496,15 +2517,15 @@
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.2">
       <c r="I21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="M21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.2">
       <c r="I22" t="s">
-        <v>56</v>
+        <v>92</v>
       </c>
       <c r="M22" s="14" t="s">
         <v>27</v>
@@ -2513,13 +2534,13 @@
     </row>
     <row r="23" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D23" s="1"/>
-      <c r="I23" s="14" t="s">
-        <v>66</v>
+      <c r="I23" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="I24" s="15" t="s">
-        <v>68</v>
+      <c r="I24" s="14" t="s">
+        <v>63</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>2</v>
@@ -2528,17 +2549,17 @@
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.2">
       <c r="I25" s="15" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="L25" s="2"/>
       <c r="M25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C26" s="2"/>
       <c r="I26" s="15" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="L26" s="2"/>
       <c r="M26" s="4"/>
@@ -2546,7 +2567,7 @@
     <row r="27" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C27" s="2"/>
       <c r="I27" s="15" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="L27" s="2"/>
       <c r="M27" s="4"/>
@@ -2555,7 +2576,9 @@
       <c r="C28" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I28" s="15"/>
+      <c r="I28" s="15" t="s">
+        <v>78</v>
+      </c>
       <c r="L28" s="2"/>
       <c r="M28" s="4"/>
     </row>
@@ -2563,19 +2586,17 @@
       <c r="D29" t="s">
         <v>32</v>
       </c>
-      <c r="H29" s="2" t="s">
+      <c r="I29" s="15"/>
+    </row>
+    <row r="30" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="H30" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="H30" s="2"/>
-      <c r="I30" s="14" t="s">
+    <row r="31" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="H31" s="2"/>
+      <c r="I31" s="14" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="3:14" x14ac:dyDescent="0.2">
-      <c r="I31" s="14" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="32" spans="3:14" x14ac:dyDescent="0.2">
@@ -2583,526 +2604,549 @@
         <v>69</v>
       </c>
     </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="I33" s="14"/>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H34" s="2" t="s">
+    <row r="33" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="I33" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="C34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I34" s="14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="35" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+      <c r="I35" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D36" t="s">
+        <v>0</v>
+      </c>
+      <c r="I36" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="37" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="I37" s="14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="I38" s="14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="39" spans="3:14" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="H40" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="I41" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="3:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="D43" t="s">
+        <v>88</v>
+      </c>
+      <c r="H43" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="I43" s="10"/>
+      <c r="J43" s="12"/>
+      <c r="L43" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="M43" s="10"/>
+      <c r="N43" s="10"/>
+    </row>
+    <row r="44" spans="3:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="D44" t="s">
+        <v>80</v>
+      </c>
+      <c r="H44" s="11"/>
+      <c r="I44" s="11"/>
+      <c r="J44" s="16"/>
+      <c r="L44" s="11"/>
+      <c r="M44" s="11"/>
+      <c r="N44" s="11"/>
+    </row>
+    <row r="45" spans="3:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="D45" t="s">
+        <v>81</v>
+      </c>
+      <c r="H45" s="11"/>
+      <c r="I45" s="11"/>
+      <c r="J45" s="16"/>
+      <c r="L45" s="11"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="11"/>
+    </row>
+    <row r="46" spans="3:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="D46" t="s">
         <v>82</v>
       </c>
-      <c r="I34" s="14"/>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C35" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I35" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D36" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D37" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="D38" t="s">
-        <v>34</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="I38" s="10"/>
-      <c r="J38" s="12"/>
-      <c r="L38" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="M38" s="10"/>
-      <c r="N38" s="10"/>
-    </row>
-    <row r="39" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="D39" t="s">
-        <v>83</v>
-      </c>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="16"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
-      <c r="N39" s="11"/>
-    </row>
-    <row r="40" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="D40" t="s">
-        <v>84</v>
-      </c>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="16"/>
-      <c r="L40" s="11"/>
-      <c r="M40" s="11"/>
-      <c r="N40" s="11"/>
-    </row>
-    <row r="41" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="D41" t="s">
-        <v>85</v>
-      </c>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="16"/>
-      <c r="L41" s="11"/>
-      <c r="M41" s="11"/>
-      <c r="N41" s="11"/>
-    </row>
-    <row r="42" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="D42" t="s">
+      <c r="H46" s="11"/>
+      <c r="I46" s="11"/>
+      <c r="J46" s="16"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="11"/>
+      <c r="N46" s="11"/>
+    </row>
+    <row r="47" spans="3:14" ht="19" x14ac:dyDescent="0.25">
+      <c r="D47" t="s">
         <v>18</v>
       </c>
-      <c r="H42" s="6"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="L42" s="6"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
-    </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D43" t="s">
+      <c r="H47" s="6"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+    </row>
+    <row r="48" spans="3:14" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
         <v>9</v>
       </c>
-      <c r="H43" s="5" t="s">
+      <c r="H48" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I43" s="5" t="s">
+      <c r="I48" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J43" s="9" t="s">
+      <c r="J48" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="L43" s="5" t="s">
+      <c r="L48" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M43" s="5" t="s">
+      <c r="M48" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="N43" s="9" t="s">
+      <c r="N48" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="D44" t="s">
+    <row r="49" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D49" t="s">
         <v>1</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="H49" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I44" s="2"/>
-      <c r="L44" s="2" t="s">
+      <c r="I49" s="2"/>
+      <c r="L49" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
-    </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
-    </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
-        <v>34</v>
-      </c>
-      <c r="D46" t="s">
-        <v>46</v>
-      </c>
-      <c r="E46" t="s">
-        <v>45</v>
-      </c>
-      <c r="F46" t="s">
-        <v>44</v>
-      </c>
-      <c r="H46" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L46" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
-        <v>34</v>
-      </c>
-      <c r="D47" t="s">
-        <v>76</v>
-      </c>
-      <c r="E47" t="s">
-        <v>77</v>
-      </c>
-      <c r="H47" s="2"/>
-      <c r="L47" s="2"/>
-    </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B48" t="s">
-        <v>34</v>
-      </c>
-      <c r="D48" t="s">
-        <v>47</v>
-      </c>
-      <c r="E48" t="s">
-        <v>67</v>
-      </c>
-      <c r="H48" t="s">
-        <v>13</v>
-      </c>
-      <c r="I48" s="1"/>
-      <c r="L48" t="s">
-        <v>13</v>
-      </c>
-      <c r="M48" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="N48" s="1"/>
-    </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B49" t="s">
-        <v>34</v>
-      </c>
-      <c r="D49" t="s">
-        <v>55</v>
-      </c>
-      <c r="H49" t="s">
-        <v>14</v>
-      </c>
-      <c r="I49" s="1"/>
-      <c r="L49" t="s">
-        <v>14</v>
-      </c>
-      <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
+      <c r="M49" s="2"/>
+      <c r="N49" s="2"/>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B50" t="s">
-        <v>34</v>
-      </c>
-      <c r="D50" t="s">
-        <v>35</v>
-      </c>
+      <c r="H50" s="2"/>
+      <c r="I50" s="2"/>
+      <c r="L50" s="2"/>
+      <c r="M50" s="2"/>
+      <c r="N50" s="2"/>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>34</v>
       </c>
       <c r="D51" t="s">
-        <v>36</v>
+        <v>45</v>
+      </c>
+      <c r="E51" t="s">
+        <v>44</v>
+      </c>
+      <c r="F51" t="s">
+        <v>43</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I51" t="s">
-        <v>17</v>
-      </c>
-      <c r="J51" t="s">
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M51" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>34</v>
+      </c>
       <c r="D52" t="s">
-        <v>19</v>
+        <v>73</v>
+      </c>
+      <c r="E52" t="s">
+        <v>74</v>
       </c>
       <c r="H52" s="2"/>
       <c r="L52" s="2"/>
     </row>
     <row r="53" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H53" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I53" s="2"/>
-      <c r="L53" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="M53" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="N53" s="2"/>
+      <c r="B53" t="s">
+        <v>34</v>
+      </c>
+      <c r="D53" t="s">
+        <v>46</v>
+      </c>
+      <c r="E53" t="s">
+        <v>64</v>
+      </c>
+      <c r="H53" t="s">
+        <v>13</v>
+      </c>
+      <c r="I53" s="1"/>
+      <c r="L53" t="s">
+        <v>13</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N53" s="1"/>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>55</v>
-      </c>
-      <c r="E54" t="s">
-        <v>57</v>
+        <v>34</v>
+      </c>
+      <c r="D54" t="s">
+        <v>54</v>
+      </c>
+      <c r="H54" t="s">
+        <v>14</v>
       </c>
       <c r="I54" s="1"/>
+      <c r="L54" t="s">
+        <v>14</v>
+      </c>
       <c r="M54" s="1"/>
       <c r="N54" s="1"/>
     </row>
     <row r="55" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>55</v>
-      </c>
-      <c r="E55" t="s">
-        <v>61</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I55" s="2"/>
-      <c r="L55" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="M55" s="2"/>
-      <c r="N55" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="D55" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="56" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
+        <v>34</v>
+      </c>
+      <c r="D56" t="s">
+        <v>36</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I56" t="s">
+        <v>17</v>
+      </c>
+      <c r="J56" t="s">
+        <v>56</v>
+      </c>
+      <c r="L56" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M56" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="57" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="D57" t="s">
+        <v>19</v>
+      </c>
+      <c r="H57" s="2"/>
+      <c r="L57" s="2"/>
+    </row>
+    <row r="58" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="H58" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I58" s="2"/>
+      <c r="L58" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M58" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="N58" s="2"/>
+    </row>
+    <row r="59" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>54</v>
+      </c>
+      <c r="E59" t="s">
         <v>55</v>
       </c>
-      <c r="E56" t="s">
-        <v>62</v>
-      </c>
-      <c r="I56" t="s">
-        <v>33</v>
-      </c>
-      <c r="M56" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="I57" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.2"/>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H59" s="2" t="s">
-        <v>2</v>
-      </c>
+      <c r="I59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
     </row>
     <row r="60" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="H60" s="2"/>
-      <c r="I60" t="s">
-        <v>78</v>
-      </c>
+      <c r="B60" t="s">
+        <v>54</v>
+      </c>
+      <c r="E60" t="s">
+        <v>59</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I60" s="2"/>
+      <c r="L60" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M60" s="2"/>
+      <c r="N60" s="2"/>
     </row>
     <row r="61" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="E61" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="62" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
-        <v>35</v>
-      </c>
-      <c r="E62" t="s">
-        <v>59</v>
-      </c>
-      <c r="H62" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="I62" s="10"/>
-      <c r="J62" s="12"/>
-    </row>
-    <row r="63" spans="2:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
-        <v>35</v>
-      </c>
-      <c r="E63" t="s">
-        <v>67</v>
-      </c>
-      <c r="H63" s="6"/>
-      <c r="I63" s="3"/>
-    </row>
+        <v>91</v>
+      </c>
+      <c r="I61" t="s">
+        <v>33</v>
+      </c>
+      <c r="M61" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="I62" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="63" spans="2:14" x14ac:dyDescent="0.2"/>
     <row r="64" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B64" t="s">
-        <v>35</v>
-      </c>
-      <c r="E64" t="s">
-        <v>60</v>
-      </c>
-      <c r="H64" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I64" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="J64" s="9" t="s">
-        <v>12</v>
+      <c r="H64" s="2" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="65" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="H65" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I65" s="2"/>
+      <c r="H65" s="2"/>
+      <c r="I65" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E66" t="s">
-        <v>87</v>
-      </c>
-      <c r="H66" s="2"/>
-      <c r="I66" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10" ht="19" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E67" t="s">
-        <v>63</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+      <c r="H67" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="I67" s="10"/>
+      <c r="J67" s="12"/>
+    </row>
+    <row r="68" spans="2:10" ht="19" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E68" t="s">
-        <v>67</v>
-      </c>
-      <c r="H68" t="s">
-        <v>13</v>
-      </c>
-      <c r="I68" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="H68" s="6"/>
+      <c r="I68" s="3"/>
     </row>
     <row r="69" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E69" t="s">
-        <v>60</v>
-      </c>
-      <c r="H69" t="s">
-        <v>14</v>
-      </c>
-      <c r="I69" s="1"/>
-    </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.2"/>
+        <v>58</v>
+      </c>
+      <c r="H69" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I69" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="J69" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H70" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I70" s="2"/>
+    </row>
     <row r="71" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E71" t="s">
-        <v>61</v>
-      </c>
-      <c r="H71" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="I71" t="s">
-        <v>17</v>
-      </c>
-      <c r="J71" t="s">
-        <v>58</v>
+        <v>84</v>
+      </c>
+      <c r="H71" s="2"/>
+      <c r="I71" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E72" t="s">
-        <v>62</v>
-      </c>
-      <c r="H72" s="2"/>
+        <v>60</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="73" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="H73" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I73" s="2"/>
+      <c r="B73" t="s">
+        <v>36</v>
+      </c>
+      <c r="E73" t="s">
+        <v>64</v>
+      </c>
+      <c r="H73" t="s">
+        <v>13</v>
+      </c>
+      <c r="I73" s="1"/>
     </row>
     <row r="74" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
-        <v>83</v>
+        <v>36</v>
       </c>
       <c r="E74" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="H75" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I75" s="2"/>
-    </row>
+        <v>58</v>
+      </c>
+      <c r="H74" t="s">
+        <v>14</v>
+      </c>
+      <c r="I74" s="1"/>
+    </row>
+    <row r="75" spans="2:10" x14ac:dyDescent="0.2"/>
     <row r="76" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E76" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="I76" t="s">
-        <v>51</v>
+        <v>17</v>
+      </c>
+      <c r="J76" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B77" t="s">
+        <v>88</v>
+      </c>
       <c r="E77" t="s">
-        <v>87</v>
-      </c>
-      <c r="I77" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="78" spans="2:10" x14ac:dyDescent="0.2"/>
+        <v>89</v>
+      </c>
+      <c r="H77" s="2"/>
+    </row>
+    <row r="78" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H78" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I78" s="2"/>
+    </row>
     <row r="79" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
+        <v>80</v>
+      </c>
+      <c r="E79" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="80" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H80" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I80" s="2"/>
+    </row>
+    <row r="81" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B81" t="s">
+        <v>81</v>
+      </c>
+      <c r="E81" t="s">
+        <v>58</v>
+      </c>
+      <c r="I81" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="82" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E82" t="s">
+        <v>84</v>
+      </c>
+      <c r="I82" s="14" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="83" spans="2:9" x14ac:dyDescent="0.2"/>
+    <row r="84" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B84" t="s">
+        <v>83</v>
+      </c>
+      <c r="D84" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="85" spans="2:9" x14ac:dyDescent="0.2"/>
+    <row r="86" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B86" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="E86" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E87" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="88" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="E88" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="D79" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="80" spans="2:10" x14ac:dyDescent="0.2"/>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B81" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="E81" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E82" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="E83" s="17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="84" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" spans="2:5" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="89" spans="2:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" spans="2:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" spans="2:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" spans="2:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" spans="2:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" spans="2:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" spans="2:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" spans="2:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="97" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="98" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="99" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3124,6 +3168,11 @@
     <row r="115" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="116" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="117" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B4:F4"/>

</xml_diff>

<commit_message>
OO Twenty One - refactoring and refinements
</commit_message>
<xml_diff>
--- a/lesson_5/oo_twenty_one/twenty_one_crc.xlsx
+++ b/lesson_5/oo_twenty_one/twenty_one_crc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jameswallace/Dropbox/Software-Projects/Launch_School/ls_rb120/lesson_5/oo_twenty_one/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{502A54B8-74D4-A144-A757-6E6C0484B691}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA54F6F-C25A-9843-9333-C7C28A9C9B17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-60260" yWindow="-28300" windowWidth="51200" windowHeight="28300" xr2:uid="{49C14D9E-246B-514D-BEB7-B27399C0C8B6}"/>
   </bookViews>
@@ -223,9 +223,6 @@
     <t>determine_winner</t>
   </si>
   <si>
-    <t>max_hand_value</t>
-  </si>
-  <si>
     <t>&gt;</t>
   </si>
   <si>
@@ -235,9 +232,6 @@
     <t>==</t>
   </si>
   <si>
-    <t>min_hand_value</t>
-  </si>
-  <si>
     <t>@hand</t>
   </si>
   <si>
@@ -329,6 +323,12 @@
   </si>
   <si>
     <t>possible_hand_values</t>
+  </si>
+  <si>
+    <t>max_playable_hand_value</t>
+  </si>
+  <si>
+    <t>min_playable_hand_value</t>
   </si>
 </sst>
 </file>
@@ -2264,7 +2264,7 @@
   <dimension ref="A1:O122"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="119" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36:E37"/>
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="14" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -2376,7 +2376,7 @@
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="M8" t="s">
         <v>52</v>
@@ -2407,7 +2407,7 @@
         <v>13</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L11" t="s">
         <v>13</v>
@@ -2475,7 +2475,7 @@
         <v>7</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="M17" s="1" t="s">
         <v>38</v>
@@ -2490,7 +2490,7 @@
         <v>30</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="3:14" x14ac:dyDescent="0.2">
@@ -2509,7 +2509,7 @@
         <v>26</v>
       </c>
       <c r="J20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M20" t="s">
         <v>6</v>
@@ -2525,7 +2525,7 @@
     </row>
     <row r="22" spans="3:14" x14ac:dyDescent="0.2">
       <c r="I22" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="M22" s="14" t="s">
         <v>27</v>
@@ -2535,12 +2535,12 @@
     <row r="23" spans="3:14" x14ac:dyDescent="0.2">
       <c r="D23" s="1"/>
       <c r="I23" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.2">
       <c r="I24" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>2</v>
@@ -2549,7 +2549,7 @@
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.2">
       <c r="I25" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="L25" s="2"/>
       <c r="M25" t="s">
@@ -2559,7 +2559,7 @@
     <row r="26" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C26" s="2"/>
       <c r="I26" s="15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L26" s="2"/>
       <c r="M26" s="4"/>
@@ -2567,7 +2567,7 @@
     <row r="27" spans="3:14" x14ac:dyDescent="0.2">
       <c r="C27" s="2"/>
       <c r="I27" s="15" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L27" s="2"/>
       <c r="M27" s="4"/>
@@ -2577,7 +2577,7 @@
         <v>3</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L28" s="2"/>
       <c r="M28" s="4"/>
@@ -2601,12 +2601,12 @@
     </row>
     <row r="32" spans="3:14" x14ac:dyDescent="0.2">
       <c r="I32" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="3:14" x14ac:dyDescent="0.2">
       <c r="I33" s="14" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="3:14" x14ac:dyDescent="0.2">
@@ -2614,7 +2614,7 @@
         <v>2</v>
       </c>
       <c r="I34" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="3:14" x14ac:dyDescent="0.2">
@@ -2622,7 +2622,7 @@
         <v>8</v>
       </c>
       <c r="I35" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="36" spans="3:14" x14ac:dyDescent="0.2">
@@ -2630,28 +2630,28 @@
         <v>0</v>
       </c>
       <c r="I36" s="14" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="3:14" x14ac:dyDescent="0.2">
       <c r="I37" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="3:14" x14ac:dyDescent="0.2">
       <c r="I38" s="14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="39" spans="3:14" x14ac:dyDescent="0.2"/>
     <row r="40" spans="3:14" x14ac:dyDescent="0.2">
       <c r="H40" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="3:14" x14ac:dyDescent="0.2">
       <c r="I41" s="14" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
     </row>
     <row r="42" spans="3:14" x14ac:dyDescent="0.2">
@@ -2661,7 +2661,7 @@
     </row>
     <row r="43" spans="3:14" ht="19" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H43" s="10" t="s">
         <v>48</v>
@@ -2676,7 +2676,7 @@
     </row>
     <row r="44" spans="3:14" ht="19" x14ac:dyDescent="0.25">
       <c r="D44" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H44" s="11"/>
       <c r="I44" s="11"/>
@@ -2687,7 +2687,7 @@
     </row>
     <row r="45" spans="3:14" ht="19" x14ac:dyDescent="0.25">
       <c r="D45" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H45" s="11"/>
       <c r="I45" s="11"/>
@@ -2698,7 +2698,7 @@
     </row>
     <row r="46" spans="3:14" ht="19" x14ac:dyDescent="0.25">
       <c r="D46" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H46" s="11"/>
       <c r="I46" s="11"/>
@@ -2787,10 +2787,10 @@
         <v>34</v>
       </c>
       <c r="D52" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E52" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H52" s="2"/>
       <c r="L52" s="2"/>
@@ -2803,7 +2803,7 @@
         <v>46</v>
       </c>
       <c r="E53" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H53" t="s">
         <v>13</v>
@@ -2918,7 +2918,7 @@
         <v>54</v>
       </c>
       <c r="E61" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I61" t="s">
         <v>33</v>
@@ -2941,7 +2941,7 @@
     <row r="65" spans="2:10" x14ac:dyDescent="0.2">
       <c r="H65" s="2"/>
       <c r="I65" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="66" spans="2:10" x14ac:dyDescent="0.2">
@@ -2949,7 +2949,7 @@
         <v>35</v>
       </c>
       <c r="E66" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="67" spans="2:10" ht="19" x14ac:dyDescent="0.25">
@@ -2970,7 +2970,7 @@
         <v>35</v>
       </c>
       <c r="E68" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H68" s="6"/>
       <c r="I68" s="3"/>
@@ -3003,11 +3003,11 @@
         <v>36</v>
       </c>
       <c r="E71" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H71" s="2"/>
       <c r="I71" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="72" spans="2:10" x14ac:dyDescent="0.2">
@@ -3026,7 +3026,7 @@
         <v>36</v>
       </c>
       <c r="E73" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H73" t="s">
         <v>13</v>
@@ -3048,7 +3048,7 @@
     <row r="75" spans="2:10" x14ac:dyDescent="0.2"/>
     <row r="76" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E76" t="s">
         <v>59</v>
@@ -3065,10 +3065,10 @@
     </row>
     <row r="77" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E77" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H77" s="2"/>
     </row>
@@ -3080,7 +3080,7 @@
     </row>
     <row r="79" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E79" t="s">
         <v>58</v>
@@ -3094,7 +3094,7 @@
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E81" t="s">
         <v>58</v>
@@ -3105,7 +3105,7 @@
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.2">
       <c r="E82" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I82" s="14" t="s">
         <v>37</v>
@@ -3114,7 +3114,7 @@
     <row r="83" spans="2:9" x14ac:dyDescent="0.2"/>
     <row r="84" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D84" s="14" t="s">
         <v>61</v>
@@ -3126,17 +3126,17 @@
         <v>61</v>
       </c>
       <c r="E86" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.2">
       <c r="E87" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="88" spans="2:9" x14ac:dyDescent="0.2">
       <c r="E88" s="17" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="89" spans="2:9" ht="14" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>